<commit_message>
Update of Nov 3rd
started working on the controller
</commit_message>
<xml_diff>
--- a/bin/Data/traderjoes.xlsx
+++ b/bin/Data/traderjoes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="963">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1435" uniqueCount="1003">
   <si>
     <t xml:space="preserve"> Phone: 205-969-7801  </t>
   </si>
@@ -2908,6 +2908,126 @@
   </si>
   <si>
     <t>WI</t>
+  </si>
+  <si>
+    <t>06811</t>
+  </si>
+  <si>
+    <t>06820</t>
+  </si>
+  <si>
+    <t>06825</t>
+  </si>
+  <si>
+    <t>06477</t>
+  </si>
+  <si>
+    <t>06905</t>
+  </si>
+  <si>
+    <t>06110</t>
+  </si>
+  <si>
+    <t>06880</t>
+  </si>
+  <si>
+    <t>04101</t>
+  </si>
+  <si>
+    <t>01720</t>
+  </si>
+  <si>
+    <t>02476</t>
+  </si>
+  <si>
+    <t>02115</t>
+  </si>
+  <si>
+    <t>02446</t>
+  </si>
+  <si>
+    <t>01803</t>
+  </si>
+  <si>
+    <t>02139</t>
+  </si>
+  <si>
+    <t>02138</t>
+  </si>
+  <si>
+    <t>02035</t>
+  </si>
+  <si>
+    <t>01701</t>
+  </si>
+  <si>
+    <t>01035</t>
+  </si>
+  <si>
+    <t>02339</t>
+  </si>
+  <si>
+    <t>02043</t>
+  </si>
+  <si>
+    <t>02601</t>
+  </si>
+  <si>
+    <t>02494</t>
+  </si>
+  <si>
+    <t>01960</t>
+  </si>
+  <si>
+    <t>01906</t>
+  </si>
+  <si>
+    <t>01545</t>
+  </si>
+  <si>
+    <t>02465</t>
+  </si>
+  <si>
+    <t>03060</t>
+  </si>
+  <si>
+    <t>03801</t>
+  </si>
+  <si>
+    <t>07012</t>
+  </si>
+  <si>
+    <t>07020</t>
+  </si>
+  <si>
+    <t>07932</t>
+  </si>
+  <si>
+    <t>08053</t>
+  </si>
+  <si>
+    <t>07041</t>
+  </si>
+  <si>
+    <t>07652</t>
+  </si>
+  <si>
+    <t>08540</t>
+  </si>
+  <si>
+    <t>07702</t>
+  </si>
+  <si>
+    <t>07470</t>
+  </si>
+  <si>
+    <t>07090</t>
+  </si>
+  <si>
+    <t>07675</t>
+  </si>
+  <si>
+    <t>05403</t>
   </si>
 </sst>
 </file>
@@ -3391,8 +3511,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3716,14 +3839,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D465"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="A433" workbookViewId="0">
+      <selection activeCell="C465" sqref="C465"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="26.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3733,7 +3857,7 @@
       <c r="B1" t="s">
         <v>921</v>
       </c>
-      <c r="C1">
+      <c r="C1" s="1">
         <v>35243</v>
       </c>
       <c r="D1" t="s">
@@ -3747,7 +3871,7 @@
       <c r="B2" t="s">
         <v>922</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>85048</v>
       </c>
       <c r="D2" t="s">
@@ -3761,7 +3885,7 @@
       <c r="B3" t="s">
         <v>922</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>85308</v>
       </c>
       <c r="D3" t="s">
@@ -3775,7 +3899,7 @@
       <c r="B4" t="s">
         <v>922</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>85204</v>
       </c>
       <c r="D4" t="s">
@@ -3789,7 +3913,7 @@
       <c r="B5" t="s">
         <v>922</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>85028</v>
       </c>
       <c r="D5" t="s">
@@ -3803,7 +3927,7 @@
       <c r="B6" t="s">
         <v>922</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>85016</v>
       </c>
       <c r="D6" t="s">
@@ -3817,7 +3941,7 @@
       <c r="B7" t="s">
         <v>922</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>86303</v>
       </c>
       <c r="D7" t="s">
@@ -3831,7 +3955,7 @@
       <c r="B8" t="s">
         <v>922</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>85253</v>
       </c>
       <c r="D8" t="s">
@@ -3845,7 +3969,7 @@
       <c r="B9" t="s">
         <v>922</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>85260</v>
       </c>
       <c r="D9" t="s">
@@ -3859,7 +3983,7 @@
       <c r="B10" t="s">
         <v>922</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>85374</v>
       </c>
       <c r="D10" t="s">
@@ -3873,7 +3997,7 @@
       <c r="B11" t="s">
         <v>922</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>85283</v>
       </c>
       <c r="D11" t="s">
@@ -3887,7 +4011,7 @@
       <c r="B12" t="s">
         <v>922</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>85719</v>
       </c>
       <c r="D12" t="s">
@@ -3901,7 +4025,7 @@
       <c r="B13" t="s">
         <v>922</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>85712</v>
       </c>
       <c r="D13" t="s">
@@ -3915,7 +4039,7 @@
       <c r="B14" t="s">
         <v>922</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <v>85712</v>
       </c>
       <c r="D14" t="s">
@@ -3929,7 +4053,7 @@
       <c r="B15" t="s">
         <v>922</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <v>85704</v>
       </c>
       <c r="D15" t="s">
@@ -3943,7 +4067,7 @@
       <c r="B16" t="s">
         <v>923</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="1">
         <v>91301</v>
       </c>
       <c r="D16" t="s">
@@ -3957,7 +4081,7 @@
       <c r="B17" t="s">
         <v>923</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="1">
         <v>94501</v>
       </c>
       <c r="D17" t="s">
@@ -3971,7 +4095,7 @@
       <c r="B18" t="s">
         <v>923</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="1">
         <v>92656</v>
       </c>
       <c r="D18" t="s">
@@ -3985,7 +4109,7 @@
       <c r="B19" t="s">
         <v>923</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="1">
         <v>93420</v>
       </c>
       <c r="D19" t="s">
@@ -3999,7 +4123,7 @@
       <c r="B20" t="s">
         <v>923</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="1">
         <v>93311</v>
       </c>
       <c r="D20" t="s">
@@ -4013,7 +4137,7 @@
       <c r="B21" t="s">
         <v>923</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="1">
         <v>94703</v>
       </c>
       <c r="D21" t="s">
@@ -4027,7 +4151,7 @@
       <c r="B22" t="s">
         <v>923</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="1">
         <v>92821</v>
       </c>
       <c r="D22" t="s">
@@ -4041,7 +4165,7 @@
       <c r="B23" t="s">
         <v>923</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="1">
         <v>94513</v>
       </c>
       <c r="D23" t="s">
@@ -4055,7 +4179,7 @@
       <c r="B24" t="s">
         <v>923</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="1">
         <v>91502</v>
       </c>
       <c r="D24" t="s">
@@ -4069,7 +4193,7 @@
       <c r="B25" t="s">
         <v>923</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="1">
         <v>93010</v>
       </c>
       <c r="D25" t="s">
@@ -4083,7 +4207,7 @@
       <c r="B26" t="s">
         <v>923</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="1">
         <v>95008</v>
       </c>
       <c r="D26" t="s">
@@ -4097,7 +4221,7 @@
       <c r="B27" t="s">
         <v>923</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="1">
         <v>95010</v>
       </c>
       <c r="D27" t="s">
@@ -4111,7 +4235,7 @@
       <c r="B28" t="s">
         <v>923</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="1">
         <v>92009</v>
       </c>
       <c r="D28" t="s">
@@ -4125,7 +4249,7 @@
       <c r="B29" t="s">
         <v>923</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="1">
         <v>94546</v>
       </c>
       <c r="D29" t="s">
@@ -4139,7 +4263,7 @@
       <c r="B30" t="s">
         <v>923</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="1">
         <v>92234</v>
       </c>
       <c r="D30" t="s">
@@ -4153,7 +4277,7 @@
       <c r="B31" t="s">
         <v>923</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="1">
         <v>90703</v>
       </c>
       <c r="D31" t="s">
@@ -4167,7 +4291,7 @@
       <c r="B32" t="s">
         <v>923</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="1">
         <v>91311</v>
       </c>
       <c r="D32" t="s">
@@ -4181,7 +4305,7 @@
       <c r="B33" t="s">
         <v>923</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="1">
         <v>95926</v>
       </c>
       <c r="D33" t="s">
@@ -4195,7 +4319,7 @@
       <c r="B34" t="s">
         <v>923</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="1">
         <v>91709</v>
       </c>
       <c r="D34" t="s">
@@ -4209,7 +4333,7 @@
       <c r="B35" t="s">
         <v>923</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="1">
         <v>91914</v>
       </c>
       <c r="D35" t="s">
@@ -4223,7 +4347,7 @@
       <c r="B36" t="s">
         <v>923</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="1">
         <v>91711</v>
       </c>
       <c r="D36" t="s">
@@ -4237,7 +4361,7 @@
       <c r="B37" t="s">
         <v>923</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="1">
         <v>93611</v>
       </c>
       <c r="D37" t="s">
@@ -4251,7 +4375,7 @@
       <c r="B38" t="s">
         <v>923</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="1">
         <v>94518</v>
       </c>
       <c r="D38" t="s">
@@ -4265,7 +4389,7 @@
       <c r="B39" t="s">
         <v>923</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="1">
         <v>94520</v>
       </c>
       <c r="D39" t="s">
@@ -4279,7 +4403,7 @@
       <c r="B40" t="s">
         <v>923</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="1">
         <v>92883</v>
       </c>
       <c r="D40" t="s">
@@ -4293,7 +4417,7 @@
       <c r="B41" t="s">
         <v>923</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="1">
         <v>92627</v>
       </c>
       <c r="D41" t="s">
@@ -4307,7 +4431,7 @@
       <c r="B42" t="s">
         <v>923</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="1">
         <v>90232</v>
       </c>
       <c r="D42" t="s">
@@ -4321,7 +4445,7 @@
       <c r="B43" t="s">
         <v>923</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="1">
         <v>90230</v>
       </c>
       <c r="D43" t="s">
@@ -4335,7 +4459,7 @@
       <c r="B44" t="s">
         <v>923</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="1">
         <v>94015</v>
       </c>
       <c r="D44" t="s">
@@ -4349,7 +4473,7 @@
       <c r="B45" t="s">
         <v>923</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="1">
         <v>94526</v>
       </c>
       <c r="D45" t="s">
@@ -4363,7 +4487,7 @@
       <c r="B46" t="s">
         <v>923</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="1">
         <v>95616</v>
       </c>
       <c r="D46" t="s">
@@ -4377,7 +4501,7 @@
       <c r="B47" t="s">
         <v>923</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="1">
         <v>92130</v>
       </c>
       <c r="D47" t="s">
@@ -4391,7 +4515,7 @@
       <c r="B48" t="s">
         <v>923</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="1">
         <v>90041</v>
       </c>
       <c r="D48" t="s">
@@ -4405,7 +4529,7 @@
       <c r="B49" t="s">
         <v>923</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="1">
         <v>94530</v>
       </c>
       <c r="D49" t="s">
@@ -4419,7 +4543,7 @@
       <c r="B50" t="s">
         <v>923</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="1">
         <v>95757</v>
       </c>
       <c r="D50" t="s">
@@ -4433,7 +4557,7 @@
       <c r="B51" t="s">
         <v>923</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="1">
         <v>94608</v>
       </c>
       <c r="D51" t="s">
@@ -4447,7 +4571,7 @@
       <c r="B52" t="s">
         <v>923</v>
       </c>
-      <c r="C52">
+      <c r="C52" s="1">
         <v>92024</v>
       </c>
       <c r="D52" t="s">
@@ -4461,7 +4585,7 @@
       <c r="B53" t="s">
         <v>923</v>
       </c>
-      <c r="C53">
+      <c r="C53" s="1">
         <v>91316</v>
       </c>
       <c r="D53" t="s">
@@ -4475,7 +4599,7 @@
       <c r="B54" t="s">
         <v>923</v>
       </c>
-      <c r="C54">
+      <c r="C54" s="1">
         <v>92025</v>
       </c>
       <c r="D54" t="s">
@@ -4489,7 +4613,7 @@
       <c r="B55" t="s">
         <v>923</v>
       </c>
-      <c r="C55">
+      <c r="C55" s="1">
         <v>95628</v>
       </c>
       <c r="D55" t="s">
@@ -4503,7 +4627,7 @@
       <c r="B56" t="s">
         <v>923</v>
       </c>
-      <c r="C56">
+      <c r="C56" s="1">
         <v>94533</v>
       </c>
       <c r="D56" t="s">
@@ -4517,7 +4641,7 @@
       <c r="B57" t="s">
         <v>923</v>
       </c>
-      <c r="C57">
+      <c r="C57" s="1">
         <v>95630</v>
       </c>
       <c r="D57" t="s">
@@ -4531,7 +4655,7 @@
       <c r="B58" t="s">
         <v>923</v>
       </c>
-      <c r="C58">
+      <c r="C58" s="1">
         <v>94538</v>
       </c>
       <c r="D58" t="s">
@@ -4545,7 +4669,7 @@
       <c r="B59" t="s">
         <v>923</v>
       </c>
-      <c r="C59">
+      <c r="C59" s="1">
         <v>93710</v>
       </c>
       <c r="D59" t="s">
@@ -4559,7 +4683,7 @@
       <c r="B60" t="s">
         <v>923</v>
       </c>
-      <c r="C60">
+      <c r="C60" s="1">
         <v>91207</v>
       </c>
       <c r="D60" t="s">
@@ -4573,7 +4697,7 @@
       <c r="B61" t="s">
         <v>923</v>
       </c>
-      <c r="C61">
+      <c r="C61" s="1">
         <v>93117</v>
       </c>
       <c r="D61" t="s">
@@ -4587,7 +4711,7 @@
       <c r="B62" t="s">
         <v>923</v>
       </c>
-      <c r="C62">
+      <c r="C62" s="1">
         <v>91344</v>
       </c>
       <c r="D62" t="s">
@@ -4601,7 +4725,7 @@
       <c r="B63" t="s">
         <v>923</v>
       </c>
-      <c r="C63">
+      <c r="C63" s="1">
         <v>90254</v>
       </c>
       <c r="D63" t="s">
@@ -4615,7 +4739,7 @@
       <c r="B64" t="s">
         <v>923</v>
       </c>
-      <c r="C64">
+      <c r="C64" s="1">
         <v>90028</v>
       </c>
       <c r="D64" t="s">
@@ -4629,7 +4753,7 @@
       <c r="B65" t="s">
         <v>923</v>
       </c>
-      <c r="C65">
+      <c r="C65" s="1">
         <v>92646</v>
       </c>
       <c r="D65" t="s">
@@ -4643,7 +4767,7 @@
       <c r="B66" t="s">
         <v>923</v>
       </c>
-      <c r="C66">
+      <c r="C66" s="1">
         <v>92648</v>
       </c>
       <c r="D66" t="s">
@@ -4657,7 +4781,7 @@
       <c r="B67" t="s">
         <v>923</v>
       </c>
-      <c r="C67">
+      <c r="C67" s="1">
         <v>92649</v>
       </c>
       <c r="D67" t="s">
@@ -4671,7 +4795,7 @@
       <c r="B68" t="s">
         <v>923</v>
       </c>
-      <c r="C68">
+      <c r="C68" s="1">
         <v>92620</v>
       </c>
       <c r="D68" t="s">
@@ -4685,7 +4809,7 @@
       <c r="B69" t="s">
         <v>923</v>
       </c>
-      <c r="C69">
+      <c r="C69" s="1">
         <v>92612</v>
       </c>
       <c r="D69" t="s">
@@ -4699,7 +4823,7 @@
       <c r="B70" t="s">
         <v>923</v>
       </c>
-      <c r="C70">
+      <c r="C70" s="1">
         <v>92604</v>
       </c>
       <c r="D70" t="s">
@@ -4713,7 +4837,7 @@
       <c r="B71" t="s">
         <v>923</v>
       </c>
-      <c r="C71">
+      <c r="C71" s="1">
         <v>91011</v>
       </c>
       <c r="D71" t="s">
@@ -4727,7 +4851,7 @@
       <c r="B72" t="s">
         <v>923</v>
       </c>
-      <c r="C72">
+      <c r="C72" s="1">
         <v>92253</v>
       </c>
       <c r="D72" t="s">
@@ -4741,7 +4865,7 @@
       <c r="B73" t="s">
         <v>923</v>
       </c>
-      <c r="C73">
+      <c r="C73" s="1">
         <v>94549</v>
       </c>
       <c r="D73" t="s">
@@ -4755,7 +4879,7 @@
       <c r="B74" t="s">
         <v>923</v>
       </c>
-      <c r="C74">
+      <c r="C74" s="1">
         <v>92653</v>
       </c>
       <c r="D74" t="s">
@@ -4769,7 +4893,7 @@
       <c r="B75" t="s">
         <v>923</v>
       </c>
-      <c r="C75">
+      <c r="C75" s="1">
         <v>92677</v>
       </c>
       <c r="D75" t="s">
@@ -4783,7 +4907,7 @@
       <c r="B76" t="s">
         <v>923</v>
       </c>
-      <c r="C76">
+      <c r="C76" s="1">
         <v>92037</v>
       </c>
       <c r="D76" t="s">
@@ -4797,7 +4921,7 @@
       <c r="B77" t="s">
         <v>923</v>
       </c>
-      <c r="C77">
+      <c r="C77" s="1">
         <v>91942</v>
       </c>
       <c r="D77" t="s">
@@ -4811,7 +4935,7 @@
       <c r="B78" t="s">
         <v>923</v>
       </c>
-      <c r="C78">
+      <c r="C78" s="1">
         <v>94921</v>
       </c>
       <c r="D78" t="s">
@@ -4825,7 +4949,7 @@
       <c r="B79" t="s">
         <v>923</v>
       </c>
-      <c r="C79">
+      <c r="C79" s="1">
         <v>94550</v>
       </c>
       <c r="D79" t="s">
@@ -4839,7 +4963,7 @@
       <c r="B80" t="s">
         <v>923</v>
       </c>
-      <c r="C80">
+      <c r="C80" s="1">
         <v>90815</v>
       </c>
       <c r="D80" t="s">
@@ -4853,7 +4977,7 @@
       <c r="B81" t="s">
         <v>923</v>
       </c>
-      <c r="C81">
+      <c r="C81" s="1">
         <v>90807</v>
       </c>
       <c r="D81" t="s">
@@ -4867,7 +4991,7 @@
       <c r="B82" t="s">
         <v>923</v>
       </c>
-      <c r="C82">
+      <c r="C82" s="1">
         <v>90803</v>
       </c>
       <c r="D82" t="s">
@@ -4881,7 +5005,7 @@
       <c r="B83" t="s">
         <v>923</v>
       </c>
-      <c r="C83">
+      <c r="C83" s="1">
         <v>94024</v>
       </c>
       <c r="D83" t="s">
@@ -4895,7 +5019,7 @@
       <c r="B84" t="s">
         <v>923</v>
       </c>
-      <c r="C84">
+      <c r="C84" s="1">
         <v>90048</v>
       </c>
       <c r="D84" t="s">
@@ -4909,7 +5033,7 @@
       <c r="B85" t="s">
         <v>923</v>
       </c>
-      <c r="C85">
+      <c r="C85" s="1">
         <v>90048</v>
       </c>
       <c r="D85" t="s">
@@ -4923,7 +5047,7 @@
       <c r="B86" t="s">
         <v>923</v>
       </c>
-      <c r="C86">
+      <c r="C86" s="1">
         <v>90036</v>
       </c>
       <c r="D86" t="s">
@@ -4937,7 +5061,7 @@
       <c r="B87" t="s">
         <v>923</v>
       </c>
-      <c r="C87">
+      <c r="C87" s="1">
         <v>90027</v>
       </c>
       <c r="D87" t="s">
@@ -4951,7 +5075,7 @@
       <c r="B88" t="s">
         <v>923</v>
       </c>
-      <c r="C88">
+      <c r="C88" s="1">
         <v>90046</v>
       </c>
       <c r="D88" t="s">
@@ -4965,7 +5089,7 @@
       <c r="B89" t="s">
         <v>923</v>
       </c>
-      <c r="C89">
+      <c r="C89" s="1">
         <v>95032</v>
       </c>
       <c r="D89" t="s">
@@ -4979,7 +5103,7 @@
       <c r="B90" t="s">
         <v>923</v>
       </c>
-      <c r="C90">
+      <c r="C90" s="1">
         <v>90266</v>
       </c>
       <c r="D90" t="s">
@@ -4993,7 +5117,7 @@
       <c r="B91" t="s">
         <v>923</v>
       </c>
-      <c r="C91">
+      <c r="C91" s="1">
         <v>90266</v>
       </c>
       <c r="D91" t="s">
@@ -5007,7 +5131,7 @@
       <c r="B92" t="s">
         <v>923</v>
       </c>
-      <c r="C92">
+      <c r="C92" s="1">
         <v>94025</v>
       </c>
       <c r="D92" t="s">
@@ -5021,7 +5145,7 @@
       <c r="B93" t="s">
         <v>923</v>
       </c>
-      <c r="C93">
+      <c r="C93" s="1">
         <v>94030</v>
       </c>
       <c r="D93" t="s">
@@ -5035,7 +5159,7 @@
       <c r="B94" t="s">
         <v>923</v>
       </c>
-      <c r="C94">
+      <c r="C94" s="1">
         <v>92105</v>
       </c>
       <c r="D94" t="s">
@@ -5049,7 +5173,7 @@
       <c r="B95" t="s">
         <v>923</v>
       </c>
-      <c r="C95">
+      <c r="C95" s="1">
         <v>92692</v>
       </c>
       <c r="D95" t="s">
@@ -5063,7 +5187,7 @@
       <c r="B96" t="s">
         <v>923</v>
       </c>
-      <c r="C96">
+      <c r="C96" s="1">
         <v>95356</v>
       </c>
       <c r="D96" t="s">
@@ -5077,7 +5201,7 @@
       <c r="B97" t="s">
         <v>923</v>
       </c>
-      <c r="C97">
+      <c r="C97" s="1">
         <v>91016</v>
       </c>
       <c r="D97" t="s">
@@ -5091,7 +5215,7 @@
       <c r="B98" t="s">
         <v>923</v>
       </c>
-      <c r="C98">
+      <c r="C98" s="1">
         <v>93940</v>
       </c>
       <c r="D98" t="s">
@@ -5105,7 +5229,7 @@
       <c r="B99" t="s">
         <v>923</v>
       </c>
-      <c r="C99">
+      <c r="C99" s="1">
         <v>91020</v>
       </c>
       <c r="D99" t="s">
@@ -5119,7 +5243,7 @@
       <c r="B100" t="s">
         <v>923</v>
       </c>
-      <c r="C100">
+      <c r="C100" s="1">
         <v>95037</v>
       </c>
       <c r="D100" t="s">
@@ -5133,7 +5257,7 @@
       <c r="B101" t="s">
         <v>923</v>
       </c>
-      <c r="C101">
+      <c r="C101" s="1">
         <v>94040</v>
       </c>
       <c r="D101" t="s">
@@ -5147,7 +5271,7 @@
       <c r="B102" t="s">
         <v>923</v>
       </c>
-      <c r="C102">
+      <c r="C102" s="1">
         <v>94558</v>
       </c>
       <c r="D102" t="s">
@@ -5161,6 +5285,9 @@
       <c r="B103" t="s">
         <v>923</v>
       </c>
+      <c r="C103" s="1">
+        <v>91320</v>
+      </c>
       <c r="D103" t="s">
         <v>204</v>
       </c>
@@ -5172,7 +5299,7 @@
       <c r="B104" t="s">
         <v>923</v>
       </c>
-      <c r="C104">
+      <c r="C104" s="1">
         <v>92657</v>
       </c>
       <c r="D104" t="s">
@@ -5186,7 +5313,7 @@
       <c r="B105" t="s">
         <v>923</v>
       </c>
-      <c r="C105">
+      <c r="C105" s="1">
         <v>94945</v>
       </c>
       <c r="D105" t="s">
@@ -5200,7 +5327,7 @@
       <c r="B106" t="s">
         <v>923</v>
       </c>
-      <c r="C106">
+      <c r="C106" s="1">
         <v>94610</v>
       </c>
       <c r="D106" t="s">
@@ -5214,7 +5341,7 @@
       <c r="B107" t="s">
         <v>923</v>
       </c>
-      <c r="C107">
+      <c r="C107" s="1">
         <v>94618</v>
       </c>
       <c r="D107" t="s">
@@ -5228,7 +5355,7 @@
       <c r="B108" t="s">
         <v>923</v>
       </c>
-      <c r="C108">
+      <c r="C108" s="1">
         <v>92054</v>
       </c>
       <c r="D108" t="s">
@@ -5242,7 +5369,7 @@
       <c r="B109" t="s">
         <v>923</v>
       </c>
-      <c r="C109">
+      <c r="C109" s="1">
         <v>92865</v>
       </c>
       <c r="D109" t="s">
@@ -5256,7 +5383,7 @@
       <c r="B110" t="s">
         <v>923</v>
       </c>
-      <c r="C110">
+      <c r="C110" s="1">
         <v>93950</v>
       </c>
       <c r="D110" t="s">
@@ -5270,7 +5397,7 @@
       <c r="B111" t="s">
         <v>923</v>
       </c>
-      <c r="C111">
+      <c r="C111" s="1">
         <v>92260</v>
       </c>
       <c r="D111" t="s">
@@ -5284,7 +5411,7 @@
       <c r="B112" t="s">
         <v>923</v>
       </c>
-      <c r="C112">
+      <c r="C112" s="1">
         <v>93551</v>
       </c>
       <c r="D112" t="s">
@@ -5298,7 +5425,7 @@
       <c r="B113" t="s">
         <v>923</v>
       </c>
-      <c r="C113">
+      <c r="C113" s="1">
         <v>94301</v>
       </c>
       <c r="D113" t="s">
@@ -5312,7 +5439,7 @@
       <c r="B114" t="s">
         <v>923</v>
       </c>
-      <c r="C114">
+      <c r="C114" s="1">
         <v>91107</v>
       </c>
       <c r="D114" t="s">
@@ -5326,7 +5453,7 @@
       <c r="B115" t="s">
         <v>923</v>
       </c>
-      <c r="C115">
+      <c r="C115" s="1">
         <v>91105</v>
       </c>
       <c r="D115" t="s">
@@ -5340,7 +5467,7 @@
       <c r="B116" t="s">
         <v>923</v>
       </c>
-      <c r="C116">
+      <c r="C116" s="1">
         <v>91101</v>
       </c>
       <c r="D116" t="s">
@@ -5354,7 +5481,7 @@
       <c r="B117" t="s">
         <v>923</v>
       </c>
-      <c r="C117">
+      <c r="C117" s="1">
         <v>94954</v>
       </c>
       <c r="D117" t="s">
@@ -5368,7 +5495,7 @@
       <c r="B118" t="s">
         <v>923</v>
       </c>
-      <c r="C118">
+      <c r="C118" s="1">
         <v>94564</v>
       </c>
       <c r="D118" t="s">
@@ -5382,7 +5509,7 @@
       <c r="B119" t="s">
         <v>923</v>
       </c>
-      <c r="C119">
+      <c r="C119" s="1">
         <v>94588</v>
       </c>
       <c r="D119" t="s">
@@ -5396,7 +5523,7 @@
       <c r="B120" t="s">
         <v>923</v>
       </c>
-      <c r="C120">
+      <c r="C120" s="1">
         <v>91737</v>
       </c>
       <c r="D120" t="s">
@@ -5410,7 +5537,7 @@
       <c r="B121" t="s">
         <v>923</v>
       </c>
-      <c r="C121">
+      <c r="C121" s="1">
         <v>90275</v>
       </c>
       <c r="D121" t="s">
@@ -5424,7 +5551,7 @@
       <c r="B122" t="s">
         <v>923</v>
       </c>
-      <c r="C122">
+      <c r="C122" s="1">
         <v>90275</v>
       </c>
       <c r="D122" t="s">
@@ -5438,7 +5565,7 @@
       <c r="B123" t="s">
         <v>923</v>
       </c>
-      <c r="C123">
+      <c r="C123" s="1">
         <v>92688</v>
       </c>
       <c r="D123" t="s">
@@ -5452,7 +5579,7 @@
       <c r="B124" t="s">
         <v>923</v>
       </c>
-      <c r="C124">
+      <c r="C124" s="1">
         <v>96003</v>
       </c>
       <c r="D124" t="s">
@@ -5466,7 +5593,7 @@
       <c r="B125" t="s">
         <v>923</v>
       </c>
-      <c r="C125">
+      <c r="C125" s="1">
         <v>92374</v>
       </c>
       <c r="D125" t="s">
@@ -5480,7 +5607,7 @@
       <c r="B126" t="s">
         <v>923</v>
       </c>
-      <c r="C126">
+      <c r="C126" s="1">
         <v>90277</v>
       </c>
       <c r="D126" t="s">
@@ -5494,7 +5621,7 @@
       <c r="B127" t="s">
         <v>923</v>
       </c>
-      <c r="C127">
+      <c r="C127" s="1">
         <v>92506</v>
       </c>
       <c r="D127" t="s">
@@ -5508,7 +5635,7 @@
       <c r="B128" t="s">
         <v>923</v>
       </c>
-      <c r="C128">
+      <c r="C128" s="1">
         <v>95678</v>
       </c>
       <c r="D128" t="s">
@@ -5522,7 +5649,7 @@
       <c r="B129" t="s">
         <v>923</v>
       </c>
-      <c r="C129">
+      <c r="C129" s="1">
         <v>95819</v>
       </c>
       <c r="D129" t="s">
@@ -5536,7 +5663,7 @@
       <c r="B130" t="s">
         <v>923</v>
       </c>
-      <c r="C130">
+      <c r="C130" s="1">
         <v>95821</v>
       </c>
       <c r="D130" t="s">
@@ -5550,7 +5677,7 @@
       <c r="B131" t="s">
         <v>923</v>
       </c>
-      <c r="C131">
+      <c r="C131" s="1">
         <v>94070</v>
       </c>
       <c r="D131" t="s">
@@ -5564,7 +5691,7 @@
       <c r="B132" t="s">
         <v>923</v>
       </c>
-      <c r="C132">
+      <c r="C132" s="1">
         <v>92673</v>
       </c>
       <c r="D132" t="s">
@@ -5578,7 +5705,7 @@
       <c r="B133" t="s">
         <v>923</v>
       </c>
-      <c r="C133">
+      <c r="C133" s="1">
         <v>92128</v>
       </c>
       <c r="D133" t="s">
@@ -5592,7 +5719,7 @@
       <c r="B134" t="s">
         <v>923</v>
       </c>
-      <c r="C134">
+      <c r="C134" s="1">
         <v>92103</v>
       </c>
       <c r="D134" t="s">
@@ -5606,7 +5733,7 @@
       <c r="B135" t="s">
         <v>923</v>
       </c>
-      <c r="C135">
+      <c r="C135" s="1">
         <v>92109</v>
       </c>
       <c r="D135" t="s">
@@ -5620,7 +5747,7 @@
       <c r="B136" t="s">
         <v>923</v>
       </c>
-      <c r="C136">
+      <c r="C136" s="1">
         <v>92106</v>
       </c>
       <c r="D136" t="s">
@@ -5634,7 +5761,7 @@
       <c r="B137" t="s">
         <v>923</v>
       </c>
-      <c r="C137">
+      <c r="C137" s="1">
         <v>92131</v>
       </c>
       <c r="D137" t="s">
@@ -5648,7 +5775,7 @@
       <c r="B138" t="s">
         <v>923</v>
       </c>
-      <c r="C138">
+      <c r="C138" s="1">
         <v>91773</v>
       </c>
       <c r="D138" t="s">
@@ -5662,7 +5789,7 @@
       <c r="B139" t="s">
         <v>923</v>
       </c>
-      <c r="C139">
+      <c r="C139" s="1">
         <v>94103</v>
       </c>
       <c r="D139" t="s">
@@ -5676,7 +5803,7 @@
       <c r="B140" t="s">
         <v>923</v>
       </c>
-      <c r="C140">
+      <c r="C140" s="1">
         <v>94118</v>
       </c>
       <c r="D140" t="s">
@@ -5690,7 +5817,7 @@
       <c r="B141" t="s">
         <v>923</v>
       </c>
-      <c r="C141">
+      <c r="C141" s="1">
         <v>94109</v>
       </c>
       <c r="D141" t="s">
@@ -5704,7 +5831,7 @@
       <c r="B142" t="s">
         <v>923</v>
       </c>
-      <c r="C142">
+      <c r="C142" s="1">
         <v>94133</v>
       </c>
       <c r="D142" t="s">
@@ -5718,7 +5845,7 @@
       <c r="B143" t="s">
         <v>923</v>
       </c>
-      <c r="C143">
+      <c r="C143" s="1">
         <v>94132</v>
       </c>
       <c r="D143" t="s">
@@ -5732,7 +5859,7 @@
       <c r="B144" t="s">
         <v>923</v>
       </c>
-      <c r="C144">
+      <c r="C144" s="1">
         <v>91775</v>
       </c>
       <c r="D144" t="s">
@@ -5746,7 +5873,7 @@
       <c r="B145" t="s">
         <v>923</v>
       </c>
-      <c r="C145">
+      <c r="C145" s="1">
         <v>95129</v>
       </c>
       <c r="D145" t="s">
@@ -5760,7 +5887,7 @@
       <c r="B146" t="s">
         <v>923</v>
       </c>
-      <c r="C146">
+      <c r="C146" s="1">
         <v>95110</v>
       </c>
       <c r="D146" t="s">
@@ -5774,7 +5901,7 @@
       <c r="B147" t="s">
         <v>923</v>
       </c>
-      <c r="C147">
+      <c r="C147" s="1">
         <v>95118</v>
       </c>
       <c r="D147" t="s">
@@ -5788,7 +5915,7 @@
       <c r="B148" t="s">
         <v>923</v>
       </c>
-      <c r="C148">
+      <c r="C148" s="1">
         <v>95110</v>
       </c>
       <c r="D148" t="s">
@@ -5802,6 +5929,9 @@
       <c r="B149" t="s">
         <v>923</v>
       </c>
+      <c r="C149" s="1">
+        <v>95118</v>
+      </c>
       <c r="D149" t="s">
         <v>292</v>
       </c>
@@ -5813,7 +5943,7 @@
       <c r="B150" t="s">
         <v>923</v>
       </c>
-      <c r="C150">
+      <c r="C150" s="1">
         <v>95129</v>
       </c>
       <c r="D150" t="s">
@@ -5827,7 +5957,7 @@
       <c r="B151" t="s">
         <v>923</v>
       </c>
-      <c r="C151">
+      <c r="C151" s="1">
         <v>93401</v>
       </c>
       <c r="D151" t="s">
@@ -5841,7 +5971,7 @@
       <c r="B152" t="s">
         <v>923</v>
       </c>
-      <c r="C152">
+      <c r="C152" s="1">
         <v>94402</v>
       </c>
       <c r="D152" t="s">
@@ -5855,7 +5985,7 @@
       <c r="B153" t="s">
         <v>923</v>
       </c>
-      <c r="C153">
+      <c r="C153" s="1">
         <v>94901</v>
       </c>
       <c r="D153" t="s">
@@ -5869,6 +5999,9 @@
       <c r="B154" t="s">
         <v>923</v>
       </c>
+      <c r="C154" s="1">
+        <v>92704</v>
+      </c>
       <c r="D154" t="s">
         <v>302</v>
       </c>
@@ -5880,7 +6013,7 @@
       <c r="B155" t="s">
         <v>923</v>
       </c>
-      <c r="C155">
+      <c r="C155" s="1">
         <v>93105</v>
       </c>
       <c r="D155" t="s">
@@ -5894,7 +6027,7 @@
       <c r="B156" t="s">
         <v>923</v>
       </c>
-      <c r="C156">
+      <c r="C156" s="1">
         <v>93103</v>
       </c>
       <c r="D156" t="s">
@@ -5908,7 +6041,7 @@
       <c r="B157" t="s">
         <v>923</v>
       </c>
-      <c r="C157">
+      <c r="C157" s="1">
         <v>95060</v>
       </c>
       <c r="D157" t="s">
@@ -5922,7 +6055,7 @@
       <c r="B158" t="s">
         <v>923</v>
       </c>
-      <c r="C158">
+      <c r="C158" s="1">
         <v>93454</v>
       </c>
       <c r="D158" t="s">
@@ -5936,7 +6069,7 @@
       <c r="B159" t="s">
         <v>923</v>
       </c>
-      <c r="C159">
+      <c r="C159" s="1">
         <v>90405</v>
       </c>
       <c r="D159" t="s">
@@ -5950,7 +6083,7 @@
       <c r="B160" t="s">
         <v>923</v>
       </c>
-      <c r="C160">
+      <c r="C160" s="1">
         <v>95403</v>
       </c>
       <c r="D160" t="s">
@@ -5964,7 +6097,7 @@
       <c r="B161" t="s">
         <v>923</v>
       </c>
-      <c r="C161">
+      <c r="C161" s="1">
         <v>95407</v>
       </c>
       <c r="D161" t="s">
@@ -5978,7 +6111,7 @@
       <c r="B162" t="s">
         <v>923</v>
       </c>
-      <c r="C162">
+      <c r="C162" s="1">
         <v>91423</v>
       </c>
       <c r="D162" t="s">
@@ -5992,7 +6125,7 @@
       <c r="B163" t="s">
         <v>923</v>
       </c>
-      <c r="C163">
+      <c r="C163" s="1">
         <v>93065</v>
       </c>
       <c r="D163" t="s">
@@ -6006,7 +6139,7 @@
       <c r="B164" t="s">
         <v>923</v>
       </c>
-      <c r="C164">
+      <c r="C164" s="1">
         <v>91030</v>
       </c>
       <c r="D164" t="s">
@@ -6020,7 +6153,7 @@
       <c r="B165" t="s">
         <v>923</v>
       </c>
-      <c r="C165">
+      <c r="C165" s="1">
         <v>94080</v>
       </c>
       <c r="D165" t="s">
@@ -6034,7 +6167,7 @@
       <c r="B166" t="s">
         <v>923</v>
       </c>
-      <c r="C166">
+      <c r="C166" s="1">
         <v>95207</v>
       </c>
       <c r="D166" t="s">
@@ -6048,7 +6181,7 @@
       <c r="B167" t="s">
         <v>923</v>
       </c>
-      <c r="C167">
+      <c r="C167" s="1">
         <v>91604</v>
       </c>
       <c r="D167" t="s">
@@ -6062,7 +6195,7 @@
       <c r="B168" t="s">
         <v>923</v>
       </c>
-      <c r="C168">
+      <c r="C168" s="1">
         <v>94087</v>
       </c>
       <c r="D168" t="s">
@@ -6076,7 +6209,7 @@
       <c r="B169" t="s">
         <v>923</v>
       </c>
-      <c r="C169">
+      <c r="C169" s="1">
         <v>92591</v>
       </c>
       <c r="D169" t="s">
@@ -6090,7 +6223,7 @@
       <c r="B170" t="s">
         <v>923</v>
       </c>
-      <c r="C170">
+      <c r="C170" s="1">
         <v>93465</v>
       </c>
       <c r="D170" t="s">
@@ -6104,7 +6237,7 @@
       <c r="B171" t="s">
         <v>923</v>
       </c>
-      <c r="C171">
+      <c r="C171" s="1">
         <v>91360</v>
       </c>
       <c r="D171" t="s">
@@ -6118,7 +6251,7 @@
       <c r="B172" t="s">
         <v>923</v>
       </c>
-      <c r="C172">
+      <c r="C172" s="1">
         <v>91602</v>
       </c>
       <c r="D172" t="s">
@@ -6132,7 +6265,7 @@
       <c r="B173" t="s">
         <v>923</v>
       </c>
-      <c r="C173">
+      <c r="C173" s="1">
         <v>90503</v>
       </c>
       <c r="D173" t="s">
@@ -6146,7 +6279,7 @@
       <c r="B174" t="s">
         <v>923</v>
       </c>
-      <c r="C174">
+      <c r="C174" s="1">
         <v>90505</v>
       </c>
       <c r="D174" t="s">
@@ -6160,7 +6293,7 @@
       <c r="B175" t="s">
         <v>923</v>
       </c>
-      <c r="C175">
+      <c r="C175" s="1">
         <v>92780</v>
       </c>
       <c r="D175" t="s">
@@ -6174,7 +6307,7 @@
       <c r="B176" t="s">
         <v>923</v>
       </c>
-      <c r="C176">
+      <c r="C176" s="1">
         <v>92780</v>
       </c>
       <c r="D176" t="s">
@@ -6188,7 +6321,7 @@
       <c r="B177" t="s">
         <v>923</v>
       </c>
-      <c r="C177">
+      <c r="C177" s="1">
         <v>91350</v>
       </c>
       <c r="D177" t="s">
@@ -6202,7 +6335,7 @@
       <c r="B178" t="s">
         <v>923</v>
       </c>
-      <c r="C178">
+      <c r="C178" s="1">
         <v>93003</v>
       </c>
       <c r="D178" t="s">
@@ -6216,7 +6349,7 @@
       <c r="B179" t="s">
         <v>923</v>
       </c>
-      <c r="C179">
+      <c r="C179" s="1">
         <v>93003</v>
       </c>
       <c r="D179" t="s">
@@ -6230,7 +6363,7 @@
       <c r="B180" t="s">
         <v>923</v>
       </c>
-      <c r="C180">
+      <c r="C180" s="1">
         <v>94596</v>
       </c>
       <c r="D180" t="s">
@@ -6244,7 +6377,7 @@
       <c r="B181" t="s">
         <v>923</v>
       </c>
-      <c r="C181">
+      <c r="C181" s="1">
         <v>91307</v>
       </c>
       <c r="D181" t="s">
@@ -6258,7 +6391,7 @@
       <c r="B182" t="s">
         <v>923</v>
       </c>
-      <c r="C182">
+      <c r="C182" s="1">
         <v>90069</v>
       </c>
       <c r="D182" t="s">
@@ -6272,7 +6405,7 @@
       <c r="B183" t="s">
         <v>923</v>
       </c>
-      <c r="C183">
+      <c r="C183" s="1">
         <v>90064</v>
       </c>
       <c r="D183" t="s">
@@ -6286,7 +6419,7 @@
       <c r="B184" t="s">
         <v>923</v>
       </c>
-      <c r="C184">
+      <c r="C184" s="1">
         <v>90034</v>
       </c>
       <c r="D184" t="s">
@@ -6300,7 +6433,7 @@
       <c r="B185" t="s">
         <v>923</v>
       </c>
-      <c r="C185">
+      <c r="C185" s="1">
         <v>90064</v>
       </c>
       <c r="D185" t="s">
@@ -6314,7 +6447,7 @@
       <c r="B186" t="s">
         <v>923</v>
       </c>
-      <c r="C186">
+      <c r="C186" s="1">
         <v>90045</v>
       </c>
       <c r="D186" t="s">
@@ -6328,7 +6461,7 @@
       <c r="B187" t="s">
         <v>923</v>
       </c>
-      <c r="C187">
+      <c r="C187" s="1">
         <v>91362</v>
       </c>
       <c r="D187" t="s">
@@ -6342,7 +6475,7 @@
       <c r="B188" t="s">
         <v>923</v>
       </c>
-      <c r="C188">
+      <c r="C188" s="1">
         <v>90024</v>
       </c>
       <c r="D188" t="s">
@@ -6356,7 +6489,7 @@
       <c r="B189" t="s">
         <v>923</v>
       </c>
-      <c r="C189">
+      <c r="C189" s="1">
         <v>90603</v>
       </c>
       <c r="D189" t="s">
@@ -6370,7 +6503,7 @@
       <c r="B190" t="s">
         <v>923</v>
       </c>
-      <c r="C190">
+      <c r="C190" s="1">
         <v>91364</v>
       </c>
       <c r="D190" t="s">
@@ -6384,7 +6517,7 @@
       <c r="B191" t="s">
         <v>923</v>
       </c>
-      <c r="C191">
+      <c r="C191" s="1">
         <v>92886</v>
       </c>
       <c r="D191" t="s">
@@ -6398,7 +6531,7 @@
       <c r="B192" t="s">
         <v>924</v>
       </c>
-      <c r="C192">
+      <c r="C192" s="1">
         <v>80301</v>
       </c>
       <c r="D192" t="s">
@@ -6412,7 +6545,7 @@
       <c r="B193" t="s">
         <v>924</v>
       </c>
-      <c r="C193">
+      <c r="C193" s="1">
         <v>80918</v>
       </c>
       <c r="D193" t="s">
@@ -6426,7 +6559,7 @@
       <c r="B194" t="s">
         <v>924</v>
       </c>
-      <c r="C194">
+      <c r="C194" s="1">
         <v>80203</v>
       </c>
       <c r="D194" t="s">
@@ -6440,7 +6573,7 @@
       <c r="B195" t="s">
         <v>924</v>
       </c>
-      <c r="C195">
+      <c r="C195" s="1">
         <v>80206</v>
       </c>
       <c r="D195" t="s">
@@ -6454,7 +6587,7 @@
       <c r="B196" t="s">
         <v>924</v>
       </c>
-      <c r="C196">
+      <c r="C196" s="1">
         <v>80525</v>
       </c>
       <c r="D196" t="s">
@@ -6468,7 +6601,7 @@
       <c r="B197" t="s">
         <v>924</v>
       </c>
-      <c r="C197">
+      <c r="C197" s="1">
         <v>80121</v>
       </c>
       <c r="D197" t="s">
@@ -6482,7 +6615,7 @@
       <c r="B198" t="s">
         <v>924</v>
       </c>
-      <c r="C198">
+      <c r="C198" s="1">
         <v>80120</v>
       </c>
       <c r="D198" t="s">
@@ -6496,8 +6629,8 @@
       <c r="B199" t="s">
         <v>925</v>
       </c>
-      <c r="C199">
-        <v>6811</v>
+      <c r="C199" s="1" t="s">
+        <v>963</v>
       </c>
       <c r="D199" t="s">
         <v>392</v>
@@ -6510,8 +6643,8 @@
       <c r="B200" t="s">
         <v>925</v>
       </c>
-      <c r="C200">
-        <v>6820</v>
+      <c r="C200" s="1" t="s">
+        <v>964</v>
       </c>
       <c r="D200" t="s">
         <v>394</v>
@@ -6524,8 +6657,8 @@
       <c r="B201" t="s">
         <v>925</v>
       </c>
-      <c r="C201">
-        <v>6825</v>
+      <c r="C201" s="1" t="s">
+        <v>965</v>
       </c>
       <c r="D201" t="s">
         <v>394</v>
@@ -6538,8 +6671,8 @@
       <c r="B202" t="s">
         <v>925</v>
       </c>
-      <c r="C202">
-        <v>6477</v>
+      <c r="C202" s="1" t="s">
+        <v>966</v>
       </c>
       <c r="D202" t="s">
         <v>397</v>
@@ -6552,8 +6685,8 @@
       <c r="B203" t="s">
         <v>925</v>
       </c>
-      <c r="C203">
-        <v>6905</v>
+      <c r="C203" s="1" t="s">
+        <v>967</v>
       </c>
       <c r="D203" t="s">
         <v>399</v>
@@ -6566,8 +6699,8 @@
       <c r="B204" t="s">
         <v>925</v>
       </c>
-      <c r="C204">
-        <v>6110</v>
+      <c r="C204" s="1" t="s">
+        <v>968</v>
       </c>
       <c r="D204" t="s">
         <v>401</v>
@@ -6580,8 +6713,8 @@
       <c r="B205" t="s">
         <v>925</v>
       </c>
-      <c r="C205">
-        <v>6880</v>
+      <c r="C205" s="1" t="s">
+        <v>969</v>
       </c>
       <c r="D205" t="s">
         <v>403</v>
@@ -6594,7 +6727,7 @@
       <c r="B206" t="s">
         <v>926</v>
       </c>
-      <c r="C206">
+      <c r="C206" s="1">
         <v>19803</v>
       </c>
       <c r="D206" t="s">
@@ -6608,7 +6741,7 @@
       <c r="B207" t="s">
         <v>927</v>
       </c>
-      <c r="C207">
+      <c r="C207" s="1">
         <v>20037</v>
       </c>
       <c r="D207" t="s">
@@ -6622,7 +6755,7 @@
       <c r="B208" t="s">
         <v>927</v>
       </c>
-      <c r="C208">
+      <c r="C208" s="1">
         <v>20009</v>
       </c>
       <c r="D208" t="s">
@@ -6636,7 +6769,7 @@
       <c r="B209" t="s">
         <v>928</v>
       </c>
-      <c r="C209">
+      <c r="C209" s="1">
         <v>33432</v>
       </c>
       <c r="D209" t="s">
@@ -6650,7 +6783,7 @@
       <c r="B210" t="s">
         <v>928</v>
       </c>
-      <c r="C210">
+      <c r="C210" s="1">
         <v>33324</v>
       </c>
       <c r="D210" t="s">
@@ -6664,7 +6797,7 @@
       <c r="B211" t="s">
         <v>928</v>
       </c>
-      <c r="C211">
+      <c r="C211" s="1">
         <v>33483</v>
       </c>
       <c r="D211" t="s">
@@ -6678,7 +6811,7 @@
       <c r="B212" t="s">
         <v>928</v>
       </c>
-      <c r="C212">
+      <c r="C212" s="1">
         <v>33304</v>
       </c>
       <c r="D212" t="s">
@@ -6692,7 +6825,7 @@
       <c r="B213" t="s">
         <v>928</v>
       </c>
-      <c r="C213">
+      <c r="C213" s="1">
         <v>32608</v>
       </c>
       <c r="D213" t="s">
@@ -6706,7 +6839,7 @@
       <c r="B214" t="s">
         <v>928</v>
       </c>
-      <c r="C214">
+      <c r="C214" s="1">
         <v>32250</v>
       </c>
       <c r="D214" t="s">
@@ -6720,7 +6853,7 @@
       <c r="B215" t="s">
         <v>928</v>
       </c>
-      <c r="C215">
+      <c r="C215" s="1">
         <v>34108</v>
       </c>
       <c r="D215" t="s">
@@ -6734,7 +6867,7 @@
       <c r="B216" t="s">
         <v>928</v>
       </c>
-      <c r="C216">
+      <c r="C216" s="1">
         <v>32819</v>
       </c>
       <c r="D216" t="s">
@@ -6748,7 +6881,7 @@
       <c r="B217" t="s">
         <v>928</v>
       </c>
-      <c r="C217">
+      <c r="C217" s="1">
         <v>33410</v>
       </c>
       <c r="D217" t="s">
@@ -6762,7 +6895,7 @@
       <c r="B218" t="s">
         <v>928</v>
       </c>
-      <c r="C218">
+      <c r="C218" s="1">
         <v>33026</v>
       </c>
       <c r="D218" t="s">
@@ -6776,7 +6909,7 @@
       <c r="B219" t="s">
         <v>928</v>
       </c>
-      <c r="C219">
+      <c r="C219" s="1">
         <v>33156</v>
       </c>
       <c r="D219" t="s">
@@ -6790,7 +6923,7 @@
       <c r="B220" t="s">
         <v>928</v>
       </c>
-      <c r="C220">
+      <c r="C220" s="1">
         <v>34231</v>
       </c>
       <c r="D220" t="s">
@@ -6804,7 +6937,7 @@
       <c r="B221" t="s">
         <v>928</v>
       </c>
-      <c r="C221">
+      <c r="C221" s="1">
         <v>33704</v>
       </c>
       <c r="D221" t="s">
@@ -6818,7 +6951,7 @@
       <c r="B222" t="s">
         <v>928</v>
       </c>
-      <c r="C222">
+      <c r="C222" s="1">
         <v>32309</v>
       </c>
       <c r="D222" t="s">
@@ -6832,7 +6965,7 @@
       <c r="B223" t="s">
         <v>928</v>
       </c>
-      <c r="C223">
+      <c r="C223" s="1">
         <v>33609</v>
       </c>
       <c r="D223" t="s">
@@ -6846,7 +6979,7 @@
       <c r="B224" t="s">
         <v>928</v>
       </c>
-      <c r="C224">
+      <c r="C224" s="1">
         <v>33414</v>
       </c>
       <c r="D224" t="s">
@@ -6860,7 +6993,7 @@
       <c r="B225" t="s">
         <v>928</v>
       </c>
-      <c r="C225">
+      <c r="C225" s="1">
         <v>32789</v>
       </c>
       <c r="D225" t="s">
@@ -6874,7 +7007,7 @@
       <c r="B226" t="s">
         <v>929</v>
       </c>
-      <c r="C226">
+      <c r="C226" s="1">
         <v>30606</v>
       </c>
       <c r="D226" t="s">
@@ -6888,7 +7021,7 @@
       <c r="B227" t="s">
         <v>929</v>
       </c>
-      <c r="C227">
+      <c r="C227" s="1">
         <v>30305</v>
       </c>
       <c r="D227" t="s">
@@ -6902,7 +7035,7 @@
       <c r="B228" t="s">
         <v>929</v>
       </c>
-      <c r="C228">
+      <c r="C228" s="1">
         <v>30308</v>
       </c>
       <c r="D228" t="s">
@@ -6916,7 +7049,7 @@
       <c r="B229" t="s">
         <v>929</v>
       </c>
-      <c r="C229">
+      <c r="C229" s="1">
         <v>30062</v>
       </c>
       <c r="D229" t="s">
@@ -6930,7 +7063,7 @@
       <c r="B230" t="s">
         <v>929</v>
       </c>
-      <c r="C230">
+      <c r="C230" s="1">
         <v>30092</v>
       </c>
       <c r="D230" t="s">
@@ -6944,7 +7077,7 @@
       <c r="B231" t="s">
         <v>929</v>
       </c>
-      <c r="C231">
+      <c r="C231" s="1">
         <v>30075</v>
       </c>
       <c r="D231" t="s">
@@ -6958,7 +7091,7 @@
       <c r="B232" t="s">
         <v>929</v>
       </c>
-      <c r="C232">
+      <c r="C232" s="1">
         <v>30328</v>
       </c>
       <c r="D232" t="s">
@@ -6972,7 +7105,7 @@
       <c r="B233" t="s">
         <v>930</v>
       </c>
-      <c r="C233">
+      <c r="C233" s="1">
         <v>83702</v>
       </c>
       <c r="D233" t="s">
@@ -6986,7 +7119,7 @@
       <c r="B234" t="s">
         <v>931</v>
       </c>
-      <c r="C234">
+      <c r="C234" s="1">
         <v>60102</v>
       </c>
       <c r="D234" t="s">
@@ -7000,7 +7133,7 @@
       <c r="B235" t="s">
         <v>931</v>
       </c>
-      <c r="C235">
+      <c r="C235" s="1">
         <v>60004</v>
       </c>
       <c r="D235" t="s">
@@ -7014,7 +7147,7 @@
       <c r="B236" t="s">
         <v>931</v>
       </c>
-      <c r="C236">
+      <c r="C236" s="1">
         <v>60510</v>
       </c>
       <c r="D236" t="s">
@@ -7028,7 +7161,7 @@
       <c r="B237" t="s">
         <v>931</v>
       </c>
-      <c r="C237">
+      <c r="C237" s="1">
         <v>60611</v>
       </c>
       <c r="D237" t="s">
@@ -7042,7 +7175,7 @@
       <c r="B238" t="s">
         <v>931</v>
       </c>
-      <c r="C238">
+      <c r="C238" s="1">
         <v>60613</v>
       </c>
       <c r="D238" t="s">
@@ -7056,7 +7189,7 @@
       <c r="B239" t="s">
         <v>931</v>
       </c>
-      <c r="C239">
+      <c r="C239" s="1">
         <v>60614</v>
       </c>
       <c r="D239" t="s">
@@ -7070,7 +7203,7 @@
       <c r="B240" t="s">
         <v>931</v>
       </c>
-      <c r="C240">
+      <c r="C240" s="1">
         <v>60605</v>
       </c>
       <c r="D240" t="s">
@@ -7084,7 +7217,7 @@
       <c r="B241" t="s">
         <v>931</v>
       </c>
-      <c r="C241">
+      <c r="C241" s="1">
         <v>60614</v>
       </c>
       <c r="D241" t="s">
@@ -7098,7 +7231,7 @@
       <c r="B242" t="s">
         <v>931</v>
       </c>
-      <c r="C242">
+      <c r="C242" s="1">
         <v>60515</v>
       </c>
       <c r="D242" t="s">
@@ -7112,7 +7245,7 @@
       <c r="B243" t="s">
         <v>931</v>
       </c>
-      <c r="C243">
+      <c r="C243" s="1">
         <v>60202</v>
       </c>
       <c r="D243" t="s">
@@ -7126,7 +7259,7 @@
       <c r="B244" t="s">
         <v>931</v>
       </c>
-      <c r="C244">
+      <c r="C244" s="1">
         <v>60137</v>
       </c>
       <c r="D244" t="s">
@@ -7140,7 +7273,7 @@
       <c r="B245" t="s">
         <v>931</v>
       </c>
-      <c r="C245">
+      <c r="C245" s="1">
         <v>60025</v>
       </c>
       <c r="D245" t="s">
@@ -7154,7 +7287,7 @@
       <c r="B246" t="s">
         <v>931</v>
       </c>
-      <c r="C246">
+      <c r="C246" s="1">
         <v>60525</v>
       </c>
       <c r="D246" t="s">
@@ -7168,7 +7301,7 @@
       <c r="B247" t="s">
         <v>931</v>
       </c>
-      <c r="C247">
+      <c r="C247" s="1">
         <v>60047</v>
       </c>
       <c r="D247" t="s">
@@ -7182,7 +7315,7 @@
       <c r="B248" t="s">
         <v>931</v>
       </c>
-      <c r="C248">
+      <c r="C248" s="1">
         <v>60540</v>
       </c>
       <c r="D248" t="s">
@@ -7196,7 +7329,7 @@
       <c r="B249" t="s">
         <v>931</v>
       </c>
-      <c r="C249">
+      <c r="C249" s="1">
         <v>60048</v>
       </c>
       <c r="D249" t="s">
@@ -7210,7 +7343,7 @@
       <c r="B250" t="s">
         <v>931</v>
       </c>
-      <c r="C250">
+      <c r="C250" s="1">
         <v>60062</v>
       </c>
       <c r="D250" t="s">
@@ -7224,7 +7357,7 @@
       <c r="B251" t="s">
         <v>931</v>
       </c>
-      <c r="C251">
+      <c r="C251" s="1">
         <v>60301</v>
       </c>
       <c r="D251" t="s">
@@ -7238,7 +7371,7 @@
       <c r="B252" t="s">
         <v>931</v>
       </c>
-      <c r="C252">
+      <c r="C252" s="1">
         <v>60462</v>
       </c>
       <c r="D252" t="s">
@@ -7252,7 +7385,7 @@
       <c r="B253" t="s">
         <v>931</v>
       </c>
-      <c r="C253">
+      <c r="C253" s="1">
         <v>60068</v>
       </c>
       <c r="D253" t="s">
@@ -7266,7 +7399,7 @@
       <c r="B254" t="s">
         <v>931</v>
       </c>
-      <c r="C254">
+      <c r="C254" s="1">
         <v>60173</v>
       </c>
       <c r="D254" t="s">
@@ -7280,7 +7413,7 @@
       <c r="B255" t="s">
         <v>932</v>
       </c>
-      <c r="C255">
+      <c r="C255" s="1">
         <v>46250</v>
       </c>
       <c r="D255" t="s">
@@ -7294,7 +7427,7 @@
       <c r="B256" t="s">
         <v>932</v>
       </c>
-      <c r="C256">
+      <c r="C256" s="1">
         <v>46268</v>
       </c>
       <c r="D256" t="s">
@@ -7308,7 +7441,7 @@
       <c r="B257" t="s">
         <v>933</v>
       </c>
-      <c r="C257">
+      <c r="C257" s="1">
         <v>50266</v>
       </c>
       <c r="D257" t="s">
@@ -7322,7 +7455,7 @@
       <c r="B258" t="s">
         <v>934</v>
       </c>
-      <c r="C258">
+      <c r="C258" s="1">
         <v>66209</v>
       </c>
       <c r="D258" t="s">
@@ -7336,7 +7469,7 @@
       <c r="B259" t="s">
         <v>935</v>
       </c>
-      <c r="C259">
+      <c r="C259" s="1">
         <v>40207</v>
       </c>
       <c r="D259" t="s">
@@ -7350,7 +7483,7 @@
       <c r="B260" t="s">
         <v>935</v>
       </c>
-      <c r="C260">
+      <c r="C260" s="1">
         <v>40503</v>
       </c>
       <c r="D260" t="s">
@@ -7364,7 +7497,7 @@
       <c r="B261" t="s">
         <v>936</v>
       </c>
-      <c r="C261">
+      <c r="C261" s="1">
         <v>70808</v>
       </c>
       <c r="D261" t="s">
@@ -7378,8 +7511,8 @@
       <c r="B262" t="s">
         <v>937</v>
       </c>
-      <c r="C262">
-        <v>4101</v>
+      <c r="C262" s="1" t="s">
+        <v>970</v>
       </c>
       <c r="D262" t="s">
         <v>516</v>
@@ -7392,7 +7525,7 @@
       <c r="B263" t="s">
         <v>938</v>
       </c>
-      <c r="C263">
+      <c r="C263" s="1">
         <v>21401</v>
       </c>
       <c r="D263" t="s">
@@ -7406,7 +7539,7 @@
       <c r="B264" t="s">
         <v>938</v>
       </c>
-      <c r="C264">
+      <c r="C264" s="1">
         <v>20815</v>
       </c>
       <c r="D264" t="s">
@@ -7420,7 +7553,7 @@
       <c r="B265" t="s">
         <v>938</v>
       </c>
-      <c r="C265">
+      <c r="C265" s="1">
         <v>21075</v>
       </c>
       <c r="D265" t="s">
@@ -7434,7 +7567,7 @@
       <c r="B266" t="s">
         <v>938</v>
       </c>
-      <c r="C266">
+      <c r="C266" s="1">
         <v>20877</v>
       </c>
       <c r="D266" t="s">
@@ -7448,7 +7581,7 @@
       <c r="B267" t="s">
         <v>938</v>
       </c>
-      <c r="C267">
+      <c r="C267" s="1">
         <v>21208</v>
       </c>
       <c r="D267" t="s">
@@ -7462,7 +7595,7 @@
       <c r="B268" t="s">
         <v>938</v>
       </c>
-      <c r="C268">
+      <c r="C268" s="1">
         <v>20852</v>
       </c>
       <c r="D268" t="s">
@@ -7476,7 +7609,7 @@
       <c r="B269" t="s">
         <v>938</v>
       </c>
-      <c r="C269">
+      <c r="C269" s="1">
         <v>20901</v>
       </c>
       <c r="D269" t="s">
@@ -7490,7 +7623,7 @@
       <c r="B270" t="s">
         <v>938</v>
       </c>
-      <c r="C270">
+      <c r="C270" s="1">
         <v>21286</v>
       </c>
       <c r="D270" t="s">
@@ -7504,8 +7637,8 @@
       <c r="B271" t="s">
         <v>939</v>
       </c>
-      <c r="C271">
-        <v>1720</v>
+      <c r="C271" s="1" t="s">
+        <v>971</v>
       </c>
       <c r="D271" t="s">
         <v>534</v>
@@ -7518,8 +7651,8 @@
       <c r="B272" t="s">
         <v>939</v>
       </c>
-      <c r="C272">
-        <v>2476</v>
+      <c r="C272" s="1" t="s">
+        <v>972</v>
       </c>
       <c r="D272" t="s">
         <v>536</v>
@@ -7532,8 +7665,8 @@
       <c r="B273" t="s">
         <v>939</v>
       </c>
-      <c r="C273">
-        <v>2115</v>
+      <c r="C273" s="1" t="s">
+        <v>973</v>
       </c>
       <c r="D273" t="s">
         <v>538</v>
@@ -7546,8 +7679,8 @@
       <c r="B274" t="s">
         <v>939</v>
       </c>
-      <c r="C274">
-        <v>2446</v>
+      <c r="C274" s="1" t="s">
+        <v>974</v>
       </c>
       <c r="D274" t="s">
         <v>540</v>
@@ -7560,8 +7693,8 @@
       <c r="B275" t="s">
         <v>939</v>
       </c>
-      <c r="C275">
-        <v>1803</v>
+      <c r="C275" s="1" t="s">
+        <v>975</v>
       </c>
       <c r="D275" t="s">
         <v>542</v>
@@ -7574,8 +7707,8 @@
       <c r="B276" t="s">
         <v>939</v>
       </c>
-      <c r="C276">
-        <v>2139</v>
+      <c r="C276" s="1" t="s">
+        <v>976</v>
       </c>
       <c r="D276" t="s">
         <v>544</v>
@@ -7588,8 +7721,8 @@
       <c r="B277" t="s">
         <v>939</v>
       </c>
-      <c r="C277">
-        <v>2138</v>
+      <c r="C277" s="1" t="s">
+        <v>977</v>
       </c>
       <c r="D277" t="s">
         <v>546</v>
@@ -7602,8 +7735,8 @@
       <c r="B278" t="s">
         <v>939</v>
       </c>
-      <c r="C278">
-        <v>2035</v>
+      <c r="C278" s="1" t="s">
+        <v>978</v>
       </c>
       <c r="D278" t="s">
         <v>548</v>
@@ -7616,8 +7749,8 @@
       <c r="B279" t="s">
         <v>939</v>
       </c>
-      <c r="C279">
-        <v>1701</v>
+      <c r="C279" s="1" t="s">
+        <v>979</v>
       </c>
       <c r="D279" t="s">
         <v>550</v>
@@ -7630,8 +7763,8 @@
       <c r="B280" t="s">
         <v>939</v>
       </c>
-      <c r="C280">
-        <v>1035</v>
+      <c r="C280" s="1" t="s">
+        <v>980</v>
       </c>
       <c r="D280" t="s">
         <v>552</v>
@@ -7644,8 +7777,8 @@
       <c r="B281" t="s">
         <v>939</v>
       </c>
-      <c r="C281">
-        <v>2339</v>
+      <c r="C281" s="1" t="s">
+        <v>981</v>
       </c>
       <c r="D281" t="s">
         <v>554</v>
@@ -7658,8 +7791,8 @@
       <c r="B282" t="s">
         <v>939</v>
       </c>
-      <c r="C282">
-        <v>2043</v>
+      <c r="C282" s="1" t="s">
+        <v>982</v>
       </c>
       <c r="D282" t="s">
         <v>556</v>
@@ -7672,8 +7805,8 @@
       <c r="B283" t="s">
         <v>939</v>
       </c>
-      <c r="C283">
-        <v>2601</v>
+      <c r="C283" s="1" t="s">
+        <v>983</v>
       </c>
       <c r="D283" t="s">
         <v>558</v>
@@ -7686,8 +7819,8 @@
       <c r="B284" t="s">
         <v>939</v>
       </c>
-      <c r="C284">
-        <v>2494</v>
+      <c r="C284" s="1" t="s">
+        <v>984</v>
       </c>
       <c r="D284" t="s">
         <v>560</v>
@@ -7700,8 +7833,8 @@
       <c r="B285" t="s">
         <v>939</v>
       </c>
-      <c r="C285">
-        <v>1960</v>
+      <c r="C285" s="1" t="s">
+        <v>985</v>
       </c>
       <c r="D285" t="s">
         <v>562</v>
@@ -7714,8 +7847,8 @@
       <c r="B286" t="s">
         <v>939</v>
       </c>
-      <c r="C286">
-        <v>1906</v>
+      <c r="C286" s="1" t="s">
+        <v>986</v>
       </c>
       <c r="D286" t="s">
         <v>563</v>
@@ -7728,8 +7861,8 @@
       <c r="B287" t="s">
         <v>939</v>
       </c>
-      <c r="C287">
-        <v>1545</v>
+      <c r="C287" s="1" t="s">
+        <v>987</v>
       </c>
       <c r="D287" t="s">
         <v>565</v>
@@ -7742,8 +7875,8 @@
       <c r="B288" t="s">
         <v>939</v>
       </c>
-      <c r="C288">
-        <v>2465</v>
+      <c r="C288" s="1" t="s">
+        <v>988</v>
       </c>
       <c r="D288" t="s">
         <v>567</v>
@@ -7756,7 +7889,7 @@
       <c r="B289" t="s">
         <v>940</v>
       </c>
-      <c r="C289">
+      <c r="C289" s="1">
         <v>48104</v>
       </c>
       <c r="D289" t="s">
@@ -7770,7 +7903,7 @@
       <c r="B290" t="s">
         <v>940</v>
       </c>
-      <c r="C290">
+      <c r="C290" s="1">
         <v>48301</v>
       </c>
       <c r="D290" t="s">
@@ -7784,7 +7917,7 @@
       <c r="B291" t="s">
         <v>940</v>
       </c>
-      <c r="C291">
+      <c r="C291" s="1">
         <v>49512</v>
       </c>
       <c r="D291" t="s">
@@ -7798,7 +7931,7 @@
       <c r="B292" t="s">
         <v>940</v>
       </c>
-      <c r="C292">
+      <c r="C292" s="1">
         <v>48230</v>
       </c>
       <c r="D292" t="s">
@@ -7812,7 +7945,7 @@
       <c r="B293" t="s">
         <v>940</v>
       </c>
-      <c r="C293">
+      <c r="C293" s="1">
         <v>48167</v>
       </c>
       <c r="D293" t="s">
@@ -7826,7 +7959,7 @@
       <c r="B294" t="s">
         <v>940</v>
       </c>
-      <c r="C294">
+      <c r="C294" s="1">
         <v>48309</v>
       </c>
       <c r="D294" t="s">
@@ -7840,7 +7973,7 @@
       <c r="B295" t="s">
         <v>940</v>
       </c>
-      <c r="C295">
+      <c r="C295" s="1">
         <v>48067</v>
       </c>
       <c r="D295" t="s">
@@ -7854,7 +7987,7 @@
       <c r="B296" t="s">
         <v>941</v>
       </c>
-      <c r="C296">
+      <c r="C296" s="1">
         <v>55435</v>
       </c>
       <c r="D296" t="s">
@@ -7868,7 +8001,7 @@
       <c r="B297" t="s">
         <v>941</v>
       </c>
-      <c r="C297">
+      <c r="C297" s="1">
         <v>55369</v>
       </c>
       <c r="D297" t="s">
@@ -7882,7 +8015,7 @@
       <c r="B298" t="s">
         <v>941</v>
       </c>
-      <c r="C298">
+      <c r="C298" s="1">
         <v>55305</v>
       </c>
       <c r="D298" t="s">
@@ -7896,7 +8029,7 @@
       <c r="B299" t="s">
         <v>941</v>
       </c>
-      <c r="C299">
+      <c r="C299" s="1">
         <v>55902</v>
       </c>
       <c r="D299" t="s">
@@ -7910,7 +8043,7 @@
       <c r="B300" t="s">
         <v>941</v>
       </c>
-      <c r="C300">
+      <c r="C300" s="1">
         <v>55126</v>
       </c>
       <c r="D300" t="s">
@@ -7924,7 +8057,7 @@
       <c r="B301" t="s">
         <v>941</v>
       </c>
-      <c r="C301">
+      <c r="C301" s="1">
         <v>55416</v>
       </c>
       <c r="D301" t="s">
@@ -7938,7 +8071,7 @@
       <c r="B302" t="s">
         <v>941</v>
       </c>
-      <c r="C302">
+      <c r="C302" s="1">
         <v>55105</v>
       </c>
       <c r="D302" t="s">
@@ -7952,7 +8085,7 @@
       <c r="B303" t="s">
         <v>941</v>
       </c>
-      <c r="C303">
+      <c r="C303" s="1">
         <v>55125</v>
       </c>
       <c r="D303" t="s">
@@ -7966,7 +8099,7 @@
       <c r="B304" t="s">
         <v>942</v>
       </c>
-      <c r="C304">
+      <c r="C304" s="1">
         <v>63144</v>
       </c>
       <c r="D304" t="s">
@@ -7980,7 +8113,7 @@
       <c r="B305" t="s">
         <v>942</v>
       </c>
-      <c r="C305">
+      <c r="C305" s="1">
         <v>63017</v>
       </c>
       <c r="D305" t="s">
@@ -7994,7 +8127,7 @@
       <c r="B306" t="s">
         <v>942</v>
       </c>
-      <c r="C306">
+      <c r="C306" s="1">
         <v>63141</v>
       </c>
       <c r="D306" t="s">
@@ -8008,7 +8141,7 @@
       <c r="B307" t="s">
         <v>942</v>
       </c>
-      <c r="C307">
+      <c r="C307" s="1">
         <v>63131</v>
       </c>
       <c r="D307" t="s">
@@ -8022,7 +8155,7 @@
       <c r="B308" t="s">
         <v>942</v>
       </c>
-      <c r="C308">
+      <c r="C308" s="1">
         <v>64114</v>
       </c>
       <c r="D308" t="s">
@@ -8036,7 +8169,7 @@
       <c r="B309" t="s">
         <v>943</v>
       </c>
-      <c r="C309">
+      <c r="C309" s="1">
         <v>68516</v>
       </c>
       <c r="D309" t="s">
@@ -8050,7 +8183,7 @@
       <c r="B310" t="s">
         <v>943</v>
       </c>
-      <c r="C310">
+      <c r="C310" s="1">
         <v>68114</v>
       </c>
       <c r="D310" t="s">
@@ -8064,7 +8197,7 @@
       <c r="B311" t="s">
         <v>944</v>
       </c>
-      <c r="C311">
+      <c r="C311" s="1">
         <v>89052</v>
       </c>
       <c r="D311" t="s">
@@ -8078,7 +8211,7 @@
       <c r="B312" t="s">
         <v>944</v>
       </c>
-      <c r="C312">
+      <c r="C312" s="1">
         <v>89705</v>
       </c>
       <c r="D312" t="s">
@@ -8092,7 +8225,7 @@
       <c r="B313" t="s">
         <v>944</v>
       </c>
-      <c r="C313">
+      <c r="C313" s="1">
         <v>89014</v>
       </c>
       <c r="D313" t="s">
@@ -8106,7 +8239,7 @@
       <c r="B314" t="s">
         <v>944</v>
       </c>
-      <c r="C314">
+      <c r="C314" s="1">
         <v>89102</v>
       </c>
       <c r="D314" t="s">
@@ -8120,7 +8253,7 @@
       <c r="B315" t="s">
         <v>944</v>
       </c>
-      <c r="C315">
+      <c r="C315" s="1">
         <v>89128</v>
       </c>
       <c r="D315" t="s">
@@ -8134,7 +8267,7 @@
       <c r="B316" t="s">
         <v>944</v>
       </c>
-      <c r="C316">
+      <c r="C316" s="1">
         <v>89135</v>
       </c>
       <c r="D316" t="s">
@@ -8148,7 +8281,7 @@
       <c r="B317" t="s">
         <v>944</v>
       </c>
-      <c r="C317">
+      <c r="C317" s="1">
         <v>89502</v>
       </c>
       <c r="D317" t="s">
@@ -8162,8 +8295,8 @@
       <c r="B318" t="s">
         <v>945</v>
       </c>
-      <c r="C318">
-        <v>3060</v>
+      <c r="C318" s="1" t="s">
+        <v>989</v>
       </c>
       <c r="D318" t="s">
         <v>627</v>
@@ -8176,8 +8309,8 @@
       <c r="B319" t="s">
         <v>945</v>
       </c>
-      <c r="C319">
-        <v>3801</v>
+      <c r="C319" s="1" t="s">
+        <v>990</v>
       </c>
       <c r="D319" t="s">
         <v>629</v>
@@ -8190,8 +8323,8 @@
       <c r="B320" t="s">
         <v>946</v>
       </c>
-      <c r="C320">
-        <v>7012</v>
+      <c r="C320" s="1" t="s">
+        <v>991</v>
       </c>
       <c r="D320" t="s">
         <v>631</v>
@@ -8204,8 +8337,8 @@
       <c r="B321" t="s">
         <v>946</v>
       </c>
-      <c r="C321">
-        <v>7020</v>
+      <c r="C321" s="1" t="s">
+        <v>992</v>
       </c>
       <c r="D321" t="s">
         <v>633</v>
@@ -8218,8 +8351,8 @@
       <c r="B322" t="s">
         <v>946</v>
       </c>
-      <c r="C322">
-        <v>7932</v>
+      <c r="C322" s="1" t="s">
+        <v>993</v>
       </c>
       <c r="D322" t="s">
         <v>635</v>
@@ -8232,8 +8365,8 @@
       <c r="B323" t="s">
         <v>946</v>
       </c>
-      <c r="C323">
-        <v>8053</v>
+      <c r="C323" s="1" t="s">
+        <v>994</v>
       </c>
       <c r="D323" t="s">
         <v>637</v>
@@ -8246,8 +8379,8 @@
       <c r="B324" t="s">
         <v>946</v>
       </c>
-      <c r="C324">
-        <v>7041</v>
+      <c r="C324" s="1" t="s">
+        <v>995</v>
       </c>
       <c r="D324" t="s">
         <v>639</v>
@@ -8260,8 +8393,8 @@
       <c r="B325" t="s">
         <v>946</v>
       </c>
-      <c r="C325">
-        <v>7652</v>
+      <c r="C325" s="1" t="s">
+        <v>996</v>
       </c>
       <c r="D325" t="s">
         <v>641</v>
@@ -8274,8 +8407,8 @@
       <c r="B326" t="s">
         <v>946</v>
       </c>
-      <c r="C326">
-        <v>8540</v>
+      <c r="C326" s="1" t="s">
+        <v>997</v>
       </c>
       <c r="D326" t="s">
         <v>643</v>
@@ -8288,8 +8421,8 @@
       <c r="B327" t="s">
         <v>946</v>
       </c>
-      <c r="C327">
-        <v>7702</v>
+      <c r="C327" s="1" t="s">
+        <v>998</v>
       </c>
       <c r="D327" t="s">
         <v>645</v>
@@ -8302,8 +8435,8 @@
       <c r="B328" t="s">
         <v>946</v>
       </c>
-      <c r="C328">
-        <v>7470</v>
+      <c r="C328" s="1" t="s">
+        <v>999</v>
       </c>
       <c r="D328" t="s">
         <v>647</v>
@@ -8316,8 +8449,8 @@
       <c r="B329" t="s">
         <v>946</v>
       </c>
-      <c r="C329">
-        <v>7090</v>
+      <c r="C329" s="1" t="s">
+        <v>1000</v>
       </c>
       <c r="D329" t="s">
         <v>649</v>
@@ -8330,8 +8463,8 @@
       <c r="B330" t="s">
         <v>946</v>
       </c>
-      <c r="C330">
-        <v>7675</v>
+      <c r="C330" s="1" t="s">
+        <v>1001</v>
       </c>
       <c r="D330" t="s">
         <v>651</v>
@@ -8344,7 +8477,7 @@
       <c r="B331" t="s">
         <v>947</v>
       </c>
-      <c r="C331">
+      <c r="C331" s="1">
         <v>87122</v>
       </c>
       <c r="D331" t="s">
@@ -8358,7 +8491,7 @@
       <c r="B332" t="s">
         <v>947</v>
       </c>
-      <c r="C332">
+      <c r="C332" s="1">
         <v>87110</v>
       </c>
       <c r="D332" t="s">
@@ -8372,7 +8505,7 @@
       <c r="B333" t="s">
         <v>947</v>
       </c>
-      <c r="C333">
+      <c r="C333" s="1">
         <v>87505</v>
       </c>
       <c r="D333" t="s">
@@ -8386,7 +8519,7 @@
       <c r="B334" t="s">
         <v>948</v>
       </c>
-      <c r="C334">
+      <c r="C334" s="1">
         <v>14228</v>
       </c>
       <c r="D334" t="s">
@@ -8400,7 +8533,7 @@
       <c r="B335" t="s">
         <v>948</v>
       </c>
-      <c r="C335">
+      <c r="C335" s="1">
         <v>11201</v>
       </c>
       <c r="D335" t="s">
@@ -8414,7 +8547,7 @@
       <c r="B336" t="s">
         <v>948</v>
       </c>
-      <c r="C336">
+      <c r="C336" s="1">
         <v>11201</v>
       </c>
       <c r="D336" t="s">
@@ -8428,7 +8561,7 @@
       <c r="B337" t="s">
         <v>948</v>
       </c>
-      <c r="C337">
+      <c r="C337" s="1">
         <v>12205</v>
       </c>
       <c r="D337" t="s">
@@ -8442,7 +8575,7 @@
       <c r="B338" t="s">
         <v>948</v>
       </c>
-      <c r="C338">
+      <c r="C338" s="1">
         <v>11725</v>
       </c>
       <c r="D338" t="s">
@@ -8456,7 +8589,7 @@
       <c r="B339" t="s">
         <v>948</v>
       </c>
-      <c r="C339">
+      <c r="C339" s="1">
         <v>11725</v>
       </c>
       <c r="D339" t="s">
@@ -8470,7 +8603,7 @@
       <c r="B340" t="s">
         <v>948</v>
       </c>
-      <c r="C340">
+      <c r="C340" s="1">
         <v>10530</v>
       </c>
       <c r="D340" t="s">
@@ -8484,7 +8617,7 @@
       <c r="B341" t="s">
         <v>948</v>
       </c>
-      <c r="C341">
+      <c r="C341" s="1">
         <v>11557</v>
       </c>
       <c r="D341" t="s">
@@ -8498,7 +8631,7 @@
       <c r="B342" t="s">
         <v>948</v>
       </c>
-      <c r="C342">
+      <c r="C342" s="1">
         <v>11755</v>
       </c>
       <c r="D342" t="s">
@@ -8512,7 +8645,7 @@
       <c r="B343" t="s">
         <v>948</v>
       </c>
-      <c r="C343">
+      <c r="C343" s="1">
         <v>10538</v>
       </c>
       <c r="D343" t="s">
@@ -8526,7 +8659,7 @@
       <c r="B344" t="s">
         <v>948</v>
       </c>
-      <c r="C344">
+      <c r="C344" s="1">
         <v>11566</v>
       </c>
       <c r="D344" t="s">
@@ -8540,7 +8673,7 @@
       <c r="B345" t="s">
         <v>948</v>
       </c>
-      <c r="C345">
+      <c r="C345" s="1">
         <v>10023</v>
       </c>
       <c r="D345" t="s">
@@ -8554,7 +8687,7 @@
       <c r="B346" t="s">
         <v>948</v>
       </c>
-      <c r="C346">
+      <c r="C346" s="1">
         <v>10016</v>
       </c>
       <c r="D346" t="s">
@@ -8568,7 +8701,7 @@
       <c r="B347" t="s">
         <v>948</v>
       </c>
-      <c r="C347">
+      <c r="C347" s="1">
         <v>10010</v>
       </c>
       <c r="D347" t="s">
@@ -8582,7 +8715,7 @@
       <c r="B348" t="s">
         <v>948</v>
       </c>
-      <c r="C348">
+      <c r="C348" s="1">
         <v>10003</v>
       </c>
       <c r="D348" t="s">
@@ -8596,7 +8729,7 @@
       <c r="B349" t="s">
         <v>948</v>
       </c>
-      <c r="C349">
+      <c r="C349" s="1">
         <v>10003</v>
       </c>
       <c r="D349" t="s">
@@ -8610,7 +8743,7 @@
       <c r="B350" t="s">
         <v>948</v>
       </c>
-      <c r="C350">
+      <c r="C350" s="1">
         <v>11572</v>
       </c>
       <c r="D350" t="s">
@@ -8624,7 +8757,7 @@
       <c r="B351" t="s">
         <v>948</v>
       </c>
-      <c r="C351">
+      <c r="C351" s="1">
         <v>11803</v>
       </c>
       <c r="D351" t="s">
@@ -8638,7 +8771,7 @@
       <c r="B352" t="s">
         <v>948</v>
       </c>
-      <c r="C352">
+      <c r="C352" s="1">
         <v>11374</v>
       </c>
       <c r="D352" t="s">
@@ -8652,7 +8785,7 @@
       <c r="B353" t="s">
         <v>948</v>
       </c>
-      <c r="C353">
+      <c r="C353" s="1">
         <v>14618</v>
       </c>
       <c r="D353" t="s">
@@ -8666,7 +8799,7 @@
       <c r="B354" t="s">
         <v>948</v>
       </c>
-      <c r="C354">
+      <c r="C354" s="1">
         <v>10583</v>
       </c>
       <c r="D354" t="s">
@@ -8680,7 +8813,7 @@
       <c r="B355" t="s">
         <v>948</v>
       </c>
-      <c r="C355">
+      <c r="C355" s="1">
         <v>10314</v>
       </c>
       <c r="D355" t="s">
@@ -8694,7 +8827,7 @@
       <c r="B356" t="s">
         <v>948</v>
       </c>
-      <c r="C356">
+      <c r="C356" s="1">
         <v>13214</v>
       </c>
       <c r="D356" t="s">
@@ -8708,7 +8841,7 @@
       <c r="B357" t="s">
         <v>948</v>
       </c>
-      <c r="C357">
+      <c r="C357" s="1">
         <v>11530</v>
       </c>
       <c r="D357" t="s">
@@ -8722,7 +8855,7 @@
       <c r="B358" t="s">
         <v>949</v>
       </c>
-      <c r="C358">
+      <c r="C358" s="1">
         <v>28801</v>
       </c>
       <c r="D358" t="s">
@@ -8736,7 +8869,7 @@
       <c r="B359" t="s">
         <v>949</v>
       </c>
-      <c r="C359">
+      <c r="C359" s="1">
         <v>27511</v>
       </c>
       <c r="D359" t="s">
@@ -8750,7 +8883,7 @@
       <c r="B360" t="s">
         <v>949</v>
       </c>
-      <c r="C360">
+      <c r="C360" s="1">
         <v>27514</v>
       </c>
       <c r="D360" t="s">
@@ -8764,7 +8897,7 @@
       <c r="B361" t="s">
         <v>949</v>
       </c>
-      <c r="C361">
+      <c r="C361" s="1">
         <v>28204</v>
       </c>
       <c r="D361" t="s">
@@ -8778,7 +8911,7 @@
       <c r="B362" t="s">
         <v>949</v>
       </c>
-      <c r="C362">
+      <c r="C362" s="1">
         <v>28262</v>
       </c>
       <c r="D362" t="s">
@@ -8792,7 +8925,7 @@
       <c r="B363" t="s">
         <v>949</v>
       </c>
-      <c r="C363">
+      <c r="C363" s="1">
         <v>28277</v>
       </c>
       <c r="D363" t="s">
@@ -8806,7 +8939,7 @@
       <c r="B364" t="s">
         <v>949</v>
       </c>
-      <c r="C364">
+      <c r="C364" s="1">
         <v>27609</v>
       </c>
       <c r="D364" t="s">
@@ -8820,7 +8953,7 @@
       <c r="B365" t="s">
         <v>949</v>
       </c>
-      <c r="C365">
+      <c r="C365" s="1">
         <v>28403</v>
       </c>
       <c r="D365" t="s">
@@ -8834,7 +8967,7 @@
       <c r="B366" t="s">
         <v>949</v>
       </c>
-      <c r="C366">
+      <c r="C366" s="1">
         <v>27103</v>
       </c>
       <c r="D366" t="s">
@@ -8848,7 +8981,7 @@
       <c r="B367" t="s">
         <v>950</v>
       </c>
-      <c r="C367">
+      <c r="C367" s="1">
         <v>45236</v>
       </c>
       <c r="D367" t="s">
@@ -8862,7 +8995,7 @@
       <c r="B368" t="s">
         <v>950</v>
       </c>
-      <c r="C368">
+      <c r="C368" s="1">
         <v>43219</v>
       </c>
       <c r="D368" t="s">
@@ -8876,7 +9009,7 @@
       <c r="B369" t="s">
         <v>950</v>
       </c>
-      <c r="C369">
+      <c r="C369" s="1">
         <v>43017</v>
       </c>
       <c r="D369" t="s">
@@ -8890,7 +9023,7 @@
       <c r="B370" t="s">
         <v>950</v>
       </c>
-      <c r="C370">
+      <c r="C370" s="1">
         <v>45429</v>
       </c>
       <c r="D370" t="s">
@@ -8904,7 +9037,7 @@
       <c r="B371" t="s">
         <v>950</v>
       </c>
-      <c r="C371">
+      <c r="C371" s="1">
         <v>44145</v>
       </c>
       <c r="D371" t="s">
@@ -8918,7 +9051,7 @@
       <c r="B372" t="s">
         <v>950</v>
       </c>
-      <c r="C372">
+      <c r="C372" s="1">
         <v>44122</v>
       </c>
       <c r="D372" t="s">
@@ -8932,7 +9065,7 @@
       <c r="B373" t="s">
         <v>951</v>
       </c>
-      <c r="C373">
+      <c r="C373" s="1">
         <v>73116</v>
       </c>
       <c r="D373" t="s">
@@ -8946,7 +9079,7 @@
       <c r="B374" t="s">
         <v>951</v>
       </c>
-      <c r="C374">
+      <c r="C374" s="1">
         <v>74105</v>
       </c>
       <c r="D374" t="s">
@@ -8960,7 +9093,7 @@
       <c r="B375" t="s">
         <v>952</v>
       </c>
-      <c r="C375">
+      <c r="C375" s="1">
         <v>97005</v>
       </c>
       <c r="D375" t="s">
@@ -8974,7 +9107,7 @@
       <c r="B376" t="s">
         <v>952</v>
       </c>
-      <c r="C376">
+      <c r="C376" s="1">
         <v>97701</v>
       </c>
       <c r="D376" t="s">
@@ -8988,7 +9121,7 @@
       <c r="B377" t="s">
         <v>952</v>
       </c>
-      <c r="C377">
+      <c r="C377" s="1">
         <v>97086</v>
       </c>
       <c r="D377" t="s">
@@ -9002,7 +9135,7 @@
       <c r="B378" t="s">
         <v>952</v>
       </c>
-      <c r="C378">
+      <c r="C378" s="1">
         <v>97330</v>
       </c>
       <c r="D378" t="s">
@@ -9016,7 +9149,7 @@
       <c r="B379" t="s">
         <v>952</v>
       </c>
-      <c r="C379">
+      <c r="C379" s="1">
         <v>97401</v>
       </c>
       <c r="D379" t="s">
@@ -9030,7 +9163,7 @@
       <c r="B380" t="s">
         <v>952</v>
       </c>
-      <c r="C380">
+      <c r="C380" s="1">
         <v>97124</v>
       </c>
       <c r="D380" t="s">
@@ -9044,7 +9177,7 @@
       <c r="B381" t="s">
         <v>952</v>
       </c>
-      <c r="C381">
+      <c r="C381" s="1">
         <v>97035</v>
       </c>
       <c r="D381" t="s">
@@ -9058,7 +9191,7 @@
       <c r="B382" t="s">
         <v>952</v>
       </c>
-      <c r="C382">
+      <c r="C382" s="1">
         <v>97501</v>
       </c>
       <c r="D382" t="s">
@@ -9072,7 +9205,7 @@
       <c r="B383" t="s">
         <v>952</v>
       </c>
-      <c r="C383">
+      <c r="C383" s="1">
         <v>97202</v>
       </c>
       <c r="D383" t="s">
@@ -9086,7 +9219,7 @@
       <c r="B384" t="s">
         <v>952</v>
       </c>
-      <c r="C384">
+      <c r="C384" s="1">
         <v>97210</v>
       </c>
       <c r="D384" t="s">
@@ -9100,7 +9233,7 @@
       <c r="B385" t="s">
         <v>952</v>
       </c>
-      <c r="C385">
+      <c r="C385" s="1">
         <v>97232</v>
       </c>
       <c r="D385" t="s">
@@ -9114,7 +9247,7 @@
       <c r="B386" t="s">
         <v>952</v>
       </c>
-      <c r="C386">
+      <c r="C386" s="1">
         <v>97302</v>
       </c>
       <c r="D386" t="s">
@@ -9128,7 +9261,7 @@
       <c r="B387" t="s">
         <v>953</v>
       </c>
-      <c r="C387">
+      <c r="C387" s="1">
         <v>19003</v>
       </c>
       <c r="D387" t="s">
@@ -9142,7 +9275,7 @@
       <c r="B388" t="s">
         <v>953</v>
       </c>
-      <c r="C388">
+      <c r="C388" s="1">
         <v>19046</v>
       </c>
       <c r="D388" t="s">
@@ -9156,7 +9289,7 @@
       <c r="B389" t="s">
         <v>953</v>
       </c>
-      <c r="C389">
+      <c r="C389" s="1">
         <v>19063</v>
       </c>
       <c r="D389" t="s">
@@ -9170,7 +9303,7 @@
       <c r="B390" t="s">
         <v>953</v>
       </c>
-      <c r="C390">
+      <c r="C390" s="1">
         <v>19454</v>
       </c>
       <c r="D390" t="s">
@@ -9184,7 +9317,7 @@
       <c r="B391" t="s">
         <v>953</v>
       </c>
-      <c r="C391">
+      <c r="C391" s="1">
         <v>19103</v>
       </c>
       <c r="D391" t="s">
@@ -9198,7 +9331,7 @@
       <c r="B392" t="s">
         <v>953</v>
       </c>
-      <c r="C392">
+      <c r="C392" s="1">
         <v>15206</v>
       </c>
       <c r="D392" t="s">
@@ -9212,7 +9345,7 @@
       <c r="B393" t="s">
         <v>953</v>
       </c>
-      <c r="C393">
+      <c r="C393" s="1">
         <v>15241</v>
       </c>
       <c r="D393" t="s">
@@ -9226,7 +9359,7 @@
       <c r="B394" t="s">
         <v>953</v>
       </c>
-      <c r="C394">
+      <c r="C394" s="1">
         <v>15237</v>
       </c>
       <c r="D394" t="s">
@@ -9240,7 +9373,7 @@
       <c r="B395" t="s">
         <v>953</v>
       </c>
-      <c r="C395">
+      <c r="C395" s="1">
         <v>16803</v>
       </c>
       <c r="D395" t="s">
@@ -9254,7 +9387,7 @@
       <c r="B396" t="s">
         <v>953</v>
       </c>
-      <c r="C396">
+      <c r="C396" s="1">
         <v>19087</v>
       </c>
       <c r="D396" t="s">
@@ -9268,7 +9401,7 @@
       <c r="B397" t="s">
         <v>954</v>
       </c>
-      <c r="C397">
+      <c r="C397" s="1">
         <v>2886</v>
       </c>
       <c r="D397" t="s">
@@ -9282,7 +9415,7 @@
       <c r="B398" t="s">
         <v>955</v>
       </c>
-      <c r="C398">
+      <c r="C398" s="1">
         <v>29206</v>
       </c>
       <c r="D398" t="s">
@@ -9296,7 +9429,7 @@
       <c r="B399" t="s">
         <v>955</v>
       </c>
-      <c r="C399">
+      <c r="C399" s="1">
         <v>29607</v>
       </c>
       <c r="D399" t="s">
@@ -9310,7 +9443,7 @@
       <c r="B400" t="s">
         <v>955</v>
       </c>
-      <c r="C400">
+      <c r="C400" s="1">
         <v>29464</v>
       </c>
       <c r="D400" t="s">
@@ -9324,7 +9457,7 @@
       <c r="B401" t="s">
         <v>956</v>
       </c>
-      <c r="C401">
+      <c r="C401" s="1">
         <v>38138</v>
       </c>
       <c r="D401" t="s">
@@ -9338,7 +9471,7 @@
       <c r="B402" t="s">
         <v>956</v>
       </c>
-      <c r="C402">
+      <c r="C402" s="1">
         <v>37215</v>
       </c>
       <c r="D402" t="s">
@@ -9352,7 +9485,7 @@
       <c r="B403" t="s">
         <v>956</v>
       </c>
-      <c r="C403">
+      <c r="C403" s="1">
         <v>37919</v>
       </c>
       <c r="D403" t="s">
@@ -9366,7 +9499,7 @@
       <c r="B404" t="s">
         <v>957</v>
       </c>
-      <c r="C404">
+      <c r="C404" s="1">
         <v>78759</v>
       </c>
       <c r="D404" t="s">
@@ -9380,7 +9513,7 @@
       <c r="B405" t="s">
         <v>957</v>
       </c>
-      <c r="C405">
+      <c r="C405" s="1">
         <v>78701</v>
       </c>
       <c r="D405" t="s">
@@ -9394,7 +9527,7 @@
       <c r="B406" t="s">
         <v>957</v>
       </c>
-      <c r="C406">
+      <c r="C406" s="1">
         <v>78746</v>
       </c>
       <c r="D406" t="s">
@@ -9408,7 +9541,7 @@
       <c r="B407" t="s">
         <v>957</v>
       </c>
-      <c r="C407">
+      <c r="C407" s="1">
         <v>75254</v>
       </c>
       <c r="D407" t="s">
@@ -9422,7 +9555,7 @@
       <c r="B408" t="s">
         <v>957</v>
       </c>
-      <c r="C408">
+      <c r="C408" s="1">
         <v>75205</v>
       </c>
       <c r="D408" t="s">
@@ -9436,7 +9569,7 @@
       <c r="B409" t="s">
         <v>957</v>
       </c>
-      <c r="C409">
+      <c r="C409" s="1">
         <v>75206</v>
       </c>
       <c r="D409" t="s">
@@ -9450,7 +9583,7 @@
       <c r="B410" t="s">
         <v>957</v>
       </c>
-      <c r="C410">
+      <c r="C410" s="1">
         <v>75230</v>
       </c>
       <c r="D410" t="s">
@@ -9464,7 +9597,7 @@
       <c r="B411" t="s">
         <v>957</v>
       </c>
-      <c r="C411">
+      <c r="C411" s="1">
         <v>75209</v>
       </c>
       <c r="D411" t="s">
@@ -9478,7 +9611,7 @@
       <c r="B412" t="s">
         <v>957</v>
       </c>
-      <c r="C412">
+      <c r="C412" s="1">
         <v>76107</v>
       </c>
       <c r="D412" t="s">
@@ -9492,7 +9625,7 @@
       <c r="B413" t="s">
         <v>957</v>
       </c>
-      <c r="C413">
+      <c r="C413" s="1">
         <v>77098</v>
       </c>
       <c r="D413" t="s">
@@ -9506,7 +9639,7 @@
       <c r="B414" t="s">
         <v>957</v>
       </c>
-      <c r="C414">
+      <c r="C414" s="1">
         <v>77057</v>
       </c>
       <c r="D414" t="s">
@@ -9520,7 +9653,7 @@
       <c r="B415" t="s">
         <v>957</v>
       </c>
-      <c r="C415">
+      <c r="C415" s="1">
         <v>77077</v>
       </c>
       <c r="D415" t="s">
@@ -9534,7 +9667,7 @@
       <c r="B416" t="s">
         <v>957</v>
       </c>
-      <c r="C416">
+      <c r="C416" s="1">
         <v>77494</v>
       </c>
       <c r="D416" t="s">
@@ -9548,7 +9681,7 @@
       <c r="B417" t="s">
         <v>957</v>
       </c>
-      <c r="C417">
+      <c r="C417" s="1">
         <v>75070</v>
       </c>
       <c r="D417" t="s">
@@ -9562,7 +9695,7 @@
       <c r="B418" t="s">
         <v>957</v>
       </c>
-      <c r="C418">
+      <c r="C418" s="1">
         <v>75093</v>
       </c>
       <c r="D418" t="s">
@@ -9576,7 +9709,7 @@
       <c r="B419" t="s">
         <v>957</v>
       </c>
-      <c r="C419">
+      <c r="C419" s="1">
         <v>78209</v>
       </c>
       <c r="D419" t="s">
@@ -9590,7 +9723,7 @@
       <c r="B420" t="s">
         <v>957</v>
       </c>
-      <c r="C420">
+      <c r="C420" s="1">
         <v>78209</v>
       </c>
       <c r="D420" t="s">
@@ -9604,7 +9737,7 @@
       <c r="B421" t="s">
         <v>957</v>
       </c>
-      <c r="C421">
+      <c r="C421" s="1">
         <v>76092</v>
       </c>
       <c r="D421" t="s">
@@ -9618,7 +9751,7 @@
       <c r="B422" t="s">
         <v>957</v>
       </c>
-      <c r="C422">
+      <c r="C422" s="1">
         <v>77381</v>
       </c>
       <c r="D422" t="s">
@@ -9632,7 +9765,7 @@
       <c r="B423" t="s">
         <v>958</v>
       </c>
-      <c r="C423">
+      <c r="C423" s="1">
         <v>84047</v>
       </c>
       <c r="D423" t="s">
@@ -9646,7 +9779,7 @@
       <c r="B424" t="s">
         <v>958</v>
       </c>
-      <c r="C424">
+      <c r="C424" s="1">
         <v>84102</v>
       </c>
       <c r="D424" t="s">
@@ -9660,8 +9793,8 @@
       <c r="B425" t="s">
         <v>959</v>
       </c>
-      <c r="C425">
-        <v>5403</v>
+      <c r="C425" s="1" t="s">
+        <v>1002</v>
       </c>
       <c r="D425" t="s">
         <v>824</v>
@@ -9674,7 +9807,7 @@
       <c r="B426" t="s">
         <v>960</v>
       </c>
-      <c r="C426">
+      <c r="C426" s="1">
         <v>22314</v>
       </c>
       <c r="D426" t="s">
@@ -9688,7 +9821,7 @@
       <c r="B427" t="s">
         <v>960</v>
       </c>
-      <c r="C427">
+      <c r="C427" s="1">
         <v>22041</v>
       </c>
       <c r="D427" t="s">
@@ -9702,7 +9835,7 @@
       <c r="B428" t="s">
         <v>960</v>
       </c>
-      <c r="C428">
+      <c r="C428" s="1">
         <v>20120</v>
       </c>
       <c r="D428" t="s">
@@ -9716,7 +9849,7 @@
       <c r="B429" t="s">
         <v>960</v>
       </c>
-      <c r="C429">
+      <c r="C429" s="1">
         <v>22901</v>
       </c>
       <c r="D429" t="s">
@@ -9730,7 +9863,7 @@
       <c r="B430" t="s">
         <v>960</v>
       </c>
-      <c r="C430">
+      <c r="C430" s="1">
         <v>22201</v>
       </c>
       <c r="D430" t="s">
@@ -9744,7 +9877,7 @@
       <c r="B431" t="s">
         <v>960</v>
       </c>
-      <c r="C431">
+      <c r="C431" s="1">
         <v>22031</v>
       </c>
       <c r="D431" t="s">
@@ -9758,7 +9891,7 @@
       <c r="B432" t="s">
         <v>960</v>
       </c>
-      <c r="C432">
+      <c r="C432" s="1">
         <v>22043</v>
       </c>
       <c r="D432" t="s">
@@ -9772,7 +9905,7 @@
       <c r="B433" t="s">
         <v>960</v>
       </c>
-      <c r="C433">
+      <c r="C433" s="1">
         <v>23602</v>
       </c>
       <c r="D433" t="s">
@@ -9786,7 +9919,7 @@
       <c r="B434" t="s">
         <v>960</v>
       </c>
-      <c r="C434">
+      <c r="C434" s="1">
         <v>20194</v>
       </c>
       <c r="D434" t="s">
@@ -9800,7 +9933,7 @@
       <c r="B435" t="s">
         <v>960</v>
       </c>
-      <c r="C435">
+      <c r="C435" s="1">
         <v>23060</v>
       </c>
       <c r="D435" t="s">
@@ -9814,7 +9947,7 @@
       <c r="B436" t="s">
         <v>960</v>
       </c>
-      <c r="C436">
+      <c r="C436" s="1">
         <v>22150</v>
       </c>
       <c r="D436" t="s">
@@ -9828,7 +9961,7 @@
       <c r="B437" t="s">
         <v>960</v>
       </c>
-      <c r="C437">
+      <c r="C437" s="1">
         <v>23454</v>
       </c>
       <c r="D437" t="s">
@@ -9842,7 +9975,7 @@
       <c r="B438" t="s">
         <v>960</v>
       </c>
-      <c r="C438">
+      <c r="C438" s="1">
         <v>23188</v>
       </c>
       <c r="D438" t="s">
@@ -9856,7 +9989,7 @@
       <c r="B439" t="s">
         <v>961</v>
       </c>
-      <c r="C439">
+      <c r="C439" s="1">
         <v>98107</v>
       </c>
       <c r="D439" t="s">
@@ -9870,7 +10003,7 @@
       <c r="B440" t="s">
         <v>961</v>
       </c>
-      <c r="C440">
+      <c r="C440" s="1">
         <v>98004</v>
       </c>
       <c r="D440" t="s">
@@ -9884,7 +10017,7 @@
       <c r="B441" t="s">
         <v>961</v>
       </c>
-      <c r="C441">
+      <c r="C441" s="1">
         <v>98007</v>
       </c>
       <c r="D441" t="s">
@@ -9898,7 +10031,7 @@
       <c r="B442" t="s">
         <v>961</v>
       </c>
-      <c r="C442">
+      <c r="C442" s="1">
         <v>98225</v>
       </c>
       <c r="D442" t="s">
@@ -9912,7 +10045,7 @@
       <c r="B443" t="s">
         <v>961</v>
       </c>
-      <c r="C443">
+      <c r="C443" s="1">
         <v>98148</v>
       </c>
       <c r="D443" t="s">
@@ -9926,7 +10059,7 @@
       <c r="B444" t="s">
         <v>961</v>
       </c>
-      <c r="C444">
+      <c r="C444" s="1">
         <v>98208</v>
       </c>
       <c r="D444" t="s">
@@ -9940,7 +10073,7 @@
       <c r="B445" t="s">
         <v>961</v>
       </c>
-      <c r="C445">
+      <c r="C445" s="1">
         <v>98003</v>
       </c>
       <c r="D445" t="s">
@@ -9954,7 +10087,7 @@
       <c r="B446" t="s">
         <v>961</v>
       </c>
-      <c r="C446">
+      <c r="C446" s="1">
         <v>98027</v>
       </c>
       <c r="D446" t="s">
@@ -9968,7 +10101,7 @@
       <c r="B447" t="s">
         <v>961</v>
       </c>
-      <c r="C447">
+      <c r="C447" s="1">
         <v>98030</v>
       </c>
       <c r="D447" t="s">
@@ -9982,7 +10115,7 @@
       <c r="B448" t="s">
         <v>961</v>
       </c>
-      <c r="C448">
+      <c r="C448" s="1">
         <v>98034</v>
       </c>
       <c r="D448" t="s">
@@ -9996,7 +10129,7 @@
       <c r="B449" t="s">
         <v>961</v>
       </c>
-      <c r="C449">
+      <c r="C449" s="1">
         <v>98036</v>
       </c>
       <c r="D449" t="s">
@@ -10010,7 +10143,7 @@
       <c r="B450" t="s">
         <v>961</v>
       </c>
-      <c r="C450">
+      <c r="C450" s="1">
         <v>98502</v>
       </c>
       <c r="D450" t="s">
@@ -10024,7 +10157,7 @@
       <c r="B451" t="s">
         <v>961</v>
       </c>
-      <c r="C451">
+      <c r="C451" s="1">
         <v>98052</v>
       </c>
       <c r="D451" t="s">
@@ -10038,7 +10171,7 @@
       <c r="B452" t="s">
         <v>961</v>
       </c>
-      <c r="C452">
+      <c r="C452" s="1">
         <v>98074</v>
       </c>
       <c r="D452" t="s">
@@ -10052,7 +10185,7 @@
       <c r="B453" t="s">
         <v>961</v>
       </c>
-      <c r="C453">
+      <c r="C453" s="1">
         <v>98105</v>
       </c>
       <c r="D453" t="s">
@@ -10066,7 +10199,7 @@
       <c r="B454" t="s">
         <v>961</v>
       </c>
-      <c r="C454">
+      <c r="C454" s="1">
         <v>98109</v>
       </c>
       <c r="D454" t="s">
@@ -10080,7 +10213,7 @@
       <c r="B455" t="s">
         <v>961</v>
       </c>
-      <c r="C455">
+      <c r="C455" s="1">
         <v>98122</v>
       </c>
       <c r="D455" t="s">
@@ -10094,7 +10227,7 @@
       <c r="B456" t="s">
         <v>961</v>
       </c>
-      <c r="C456">
+      <c r="C456" s="1">
         <v>98116</v>
       </c>
       <c r="D456" t="s">
@@ -10108,7 +10241,7 @@
       <c r="B457" t="s">
         <v>961</v>
       </c>
-      <c r="C457">
+      <c r="C457" s="1">
         <v>98133</v>
       </c>
       <c r="D457" t="s">
@@ -10122,7 +10255,7 @@
       <c r="B458" t="s">
         <v>961</v>
       </c>
-      <c r="C458">
+      <c r="C458" s="1">
         <v>98383</v>
       </c>
       <c r="D458" t="s">
@@ -10136,7 +10269,7 @@
       <c r="B459" t="s">
         <v>961</v>
       </c>
-      <c r="C459">
+      <c r="C459" s="1">
         <v>99223</v>
       </c>
       <c r="D459" t="s">
@@ -10150,7 +10283,7 @@
       <c r="B460" t="s">
         <v>961</v>
       </c>
-      <c r="C460">
+      <c r="C460" s="1">
         <v>99208</v>
       </c>
       <c r="D460" t="s">
@@ -10164,7 +10297,7 @@
       <c r="B461" t="s">
         <v>961</v>
       </c>
-      <c r="C461">
+      <c r="C461" s="1">
         <v>98466</v>
       </c>
       <c r="D461" t="s">
@@ -10178,7 +10311,7 @@
       <c r="B462" t="s">
         <v>961</v>
       </c>
-      <c r="C462">
+      <c r="C462" s="1">
         <v>98683</v>
       </c>
       <c r="D462" t="s">
@@ -10192,7 +10325,7 @@
       <c r="B463" t="s">
         <v>962</v>
       </c>
-      <c r="C463">
+      <c r="C463" s="1">
         <v>53005</v>
       </c>
       <c r="D463" t="s">
@@ -10206,7 +10339,7 @@
       <c r="B464" t="s">
         <v>962</v>
       </c>
-      <c r="C464">
+      <c r="C464" s="1">
         <v>53217</v>
       </c>
       <c r="D464" t="s">
@@ -10220,7 +10353,7 @@
       <c r="B465" t="s">
         <v>962</v>
       </c>
-      <c r="C465">
+      <c r="C465" s="1">
         <v>53711</v>
       </c>
       <c r="D465" t="s">
@@ -10229,5 +10362,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>